<commit_message>
Update files and calendar (2025-10-02 17:29:24 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29325"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{A7D92622-B2E5-4E59-B8B9-C627DE387794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2040,24 +2040,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2094,13 +2076,31 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2737,43 +2737,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="163" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-      <c r="AF1" s="163"/>
+      <c r="A1" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="157"/>
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="157"/>
+      <c r="AF1" s="157"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2869,19 +2869,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
-      <c r="AL2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="160"/>
-      <c r="AN2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
+      <c r="AL2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="172"/>
+      <c r="AN2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4231,15 +4231,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4261,29 +4261,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4305,27 +4305,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4347,27 +4347,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4659,6 +4659,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4666,12 +4672,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4687,9 +4687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439DF5C5-7B05-42AC-912E-093F75C23909}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AH13" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AH13" sqref="AH13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -4744,7 +4744,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4840,14 +4840,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -4961,8 +4961,8 @@
       <c r="C4" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="72" t="s">
-        <v>16</v>
+      <c r="D4" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
@@ -5054,11 +5054,11 @@
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -6223,15 +6223,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6253,29 +6253,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6297,27 +6297,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6339,27 +6339,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6734,7 +6734,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6827,14 +6827,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7031,7 +7031,7 @@
       </c>
       <c r="AG4" s="1">
         <f>'OCT25'!AJ4</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AH4" s="1">
         <f>COUNTIF(B4:AE4,"U")</f>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="AI4" s="1">
         <f t="shared" ref="AI4:AI11" si="0">AG4-AH4</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1">
@@ -8171,15 +8171,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8201,29 +8201,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8245,27 +8245,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8287,27 +8287,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8626,8 +8626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DFC48C-09FC-43B2-ADD0-28180192959C}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -8683,7 +8683,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8779,14 +8779,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -8989,7 +8989,7 @@
       </c>
       <c r="AH4" s="1">
         <f>'NOV25'!AI4</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -10162,15 +10162,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10192,29 +10192,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10236,27 +10236,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10278,27 +10278,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10641,40 +10641,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
+      <c r="A1" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="176"/>
+      <c r="W1" s="176"/>
+      <c r="X1" s="176"/>
+      <c r="Y1" s="176"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10761,19 +10761,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="160"/>
-      <c r="AG2" s="161"/>
-      <c r="AI2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="160"/>
-      <c r="AK2" s="161"/>
+      <c r="AE2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="173"/>
+      <c r="AI2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -12023,15 +12023,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12053,29 +12053,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12097,27 +12097,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12139,27 +12139,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12451,6 +12451,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12459,11 +12464,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12539,7 +12539,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12635,19 +12635,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
-      <c r="AL2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="160"/>
-      <c r="AN2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
+      <c r="AL2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="172"/>
+      <c r="AN2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -14009,15 +14009,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14051,15 +14051,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14093,15 +14093,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14135,15 +14135,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14521,7 +14521,7 @@
       <c r="AE1" s="178"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14614,19 +14614,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
-      <c r="AK2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="160"/>
-      <c r="AM2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
+      <c r="AK2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="172"/>
+      <c r="AM2" s="173"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15947,15 +15947,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15989,15 +15989,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16031,15 +16031,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16073,15 +16073,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16373,6 +16373,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16380,11 +16385,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16457,7 +16457,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16553,14 +16553,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17831,15 +17831,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17861,29 +17861,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17905,27 +17905,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17947,27 +17947,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18259,18 +18259,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AB19:AH21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18306,42 +18306,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
+      <c r="A1" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="176"/>
+      <c r="W1" s="176"/>
+      <c r="X1" s="176"/>
+      <c r="Y1" s="176"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="176"/>
+      <c r="AB1" s="176"/>
+      <c r="AC1" s="176"/>
+      <c r="AD1" s="176"/>
+      <c r="AE1" s="176"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18434,14 +18434,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19675,15 +19675,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19710,15 +19710,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19745,15 +19745,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19780,15 +19780,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20164,7 +20164,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20260,14 +20260,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21567,15 +21567,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21602,15 +21602,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21637,15 +21637,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21672,15 +21672,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22055,7 +22055,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22151,14 +22151,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23428,15 +23428,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23458,29 +23458,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23502,27 +23502,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23544,27 +23544,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23942,7 +23942,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -24035,14 +24035,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25364,15 +25364,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25394,29 +25394,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25438,27 +25438,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25480,27 +25480,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25830,6 +25830,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="498ada7362b9f367b0ad53f1b26877d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1476f59a5677fe7b272908915e2ed05" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26064,70 +26126,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26135,5 +26135,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-10-07 17:31:42 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29401"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{A7D92622-B2E5-4E59-B8B9-C627DE387794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2040,6 +2040,24 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2076,31 +2094,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2737,43 +2737,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="157" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
-      <c r="J1" s="157"/>
-      <c r="K1" s="157"/>
-      <c r="L1" s="157"/>
-      <c r="M1" s="157"/>
-      <c r="N1" s="157"/>
-      <c r="O1" s="157"/>
-      <c r="P1" s="157"/>
-      <c r="Q1" s="157"/>
-      <c r="R1" s="157"/>
-      <c r="S1" s="157"/>
-      <c r="T1" s="157"/>
-      <c r="U1" s="157"/>
-      <c r="V1" s="157"/>
-      <c r="W1" s="157"/>
-      <c r="X1" s="157"/>
-      <c r="Y1" s="157"/>
-      <c r="Z1" s="157"/>
-      <c r="AA1" s="157"/>
-      <c r="AB1" s="157"/>
-      <c r="AC1" s="157"/>
-      <c r="AD1" s="157"/>
-      <c r="AE1" s="157"/>
-      <c r="AF1" s="157"/>
+      <c r="A1" s="163" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
+      <c r="AF1" s="163"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2869,19 +2869,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
-      <c r="AL2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
+      <c r="AL2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="160"/>
+      <c r="AN2" s="161"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4231,15 +4231,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4261,29 +4261,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="167"/>
+      <c r="AD19" s="167"/>
+      <c r="AE19" s="167"/>
+      <c r="AF19" s="167"/>
+      <c r="AG19" s="167"/>
+      <c r="AH19" s="168"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4305,27 +4305,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="169"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4347,27 +4347,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4659,12 +4659,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4672,6 +4666,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4689,7 +4689,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -4744,7 +4744,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4840,14 +4840,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="175"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -5324,11 +5324,11 @@
       <c r="N7" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="82" t="s">
-        <v>23</v>
+      <c r="O7" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>17</v>
@@ -5384,11 +5384,11 @@
       </c>
       <c r="AI7" s="1">
         <f>COUNTIF(B7:AF7,"U")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="15" customHeight="1">
@@ -6149,11 +6149,11 @@
       </c>
       <c r="O15" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="70">
         <f t="shared" si="5"/>
@@ -6223,15 +6223,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6253,29 +6253,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6297,27 +6297,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6339,27 +6339,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="172"/>
+      <c r="AC22" s="173"/>
+      <c r="AD22" s="173"/>
+      <c r="AE22" s="173"/>
+      <c r="AF22" s="173"/>
+      <c r="AG22" s="173"/>
+      <c r="AH22" s="174"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="158"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6679,7 +6679,7 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AI17" sqref="AI17"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -6734,7 +6734,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6827,14 +6827,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="160"/>
+      <c r="AI2" s="161"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7352,7 +7352,7 @@
       </c>
       <c r="AG7" s="1">
         <f>'OCT25'!AJ7</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" si="1"/>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="AI7" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1">
@@ -8171,15 +8171,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8201,29 +8201,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8245,27 +8245,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8287,27 +8287,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="172"/>
+      <c r="AC22" s="173"/>
+      <c r="AD22" s="173"/>
+      <c r="AE22" s="173"/>
+      <c r="AF22" s="173"/>
+      <c r="AG22" s="173"/>
+      <c r="AH22" s="174"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="158"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8627,8 +8627,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8683,7 +8683,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8779,14 +8779,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="175"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="AH7" s="1">
         <f>'NOV25'!AI7</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="1">
         <f>COUNTIF(B7:AF7,"U")</f>
@@ -9327,7 +9327,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="15" customHeight="1">
@@ -10162,15 +10162,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10192,29 +10192,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10236,27 +10236,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10278,27 +10278,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="172"/>
+      <c r="AC22" s="173"/>
+      <c r="AD22" s="173"/>
+      <c r="AE22" s="173"/>
+      <c r="AF22" s="173"/>
+      <c r="AG22" s="173"/>
+      <c r="AH22" s="174"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="158"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10641,40 +10641,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="175" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="175"/>
-      <c r="AB1" s="175"/>
-      <c r="AC1" s="175"/>
+      <c r="A1" s="176" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="176"/>
+      <c r="AB1" s="176"/>
+      <c r="AC1" s="176"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10761,19 +10761,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="173"/>
-      <c r="AI2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="173"/>
+      <c r="AE2" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="160"/>
+      <c r="AG2" s="161"/>
+      <c r="AI2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="160"/>
+      <c r="AK2" s="161"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="175"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -12023,15 +12023,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12053,29 +12053,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="167"/>
+      <c r="AD19" s="167"/>
+      <c r="AE19" s="167"/>
+      <c r="AF19" s="167"/>
+      <c r="AG19" s="167"/>
+      <c r="AH19" s="168"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12097,27 +12097,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="169"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12139,27 +12139,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12451,11 +12451,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12464,6 +12459,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12539,7 +12539,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12635,19 +12635,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
-      <c r="AL2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
+      <c r="AL2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="160"/>
+      <c r="AN2" s="161"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -14009,15 +14009,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14051,15 +14051,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14093,15 +14093,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14135,15 +14135,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14521,7 +14521,7 @@
       <c r="AE1" s="178"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14614,19 +14614,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
-      <c r="AK2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="172"/>
-      <c r="AM2" s="173"/>
+      <c r="AG2" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="160"/>
+      <c r="AI2" s="161"/>
+      <c r="AK2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="160"/>
+      <c r="AM2" s="161"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15947,15 +15947,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15989,15 +15989,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16031,15 +16031,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16073,15 +16073,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16373,11 +16373,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16385,6 +16380,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16457,7 +16457,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16553,14 +16553,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17831,15 +17831,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17861,29 +17861,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="167"/>
+      <c r="AD19" s="167"/>
+      <c r="AE19" s="167"/>
+      <c r="AF19" s="167"/>
+      <c r="AG19" s="167"/>
+      <c r="AH19" s="168"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17905,27 +17905,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="169"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17947,27 +17947,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18259,18 +18259,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18306,42 +18306,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="175" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
+      <c r="A1" s="176" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18434,14 +18434,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="160"/>
+      <c r="AI2" s="161"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19675,15 +19675,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19710,15 +19710,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19745,15 +19745,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19780,15 +19780,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20164,7 +20164,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20260,14 +20260,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21567,15 +21567,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21602,15 +21602,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21637,15 +21637,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21672,15 +21672,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="158"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22055,7 +22055,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22151,14 +22151,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="160"/>
+      <c r="AJ2" s="161"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="175"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23428,15 +23428,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="162"/>
+      <c r="H19" s="162"/>
+      <c r="I19" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23458,29 +23458,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="167"/>
+      <c r="AD19" s="167"/>
+      <c r="AE19" s="167"/>
+      <c r="AF19" s="167"/>
+      <c r="AG19" s="167"/>
+      <c r="AH19" s="168"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="158"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23502,27 +23502,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="169"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23544,27 +23544,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23942,7 +23942,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="164">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -24035,14 +24035,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="160"/>
+      <c r="AI2" s="161"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25364,15 +25364,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25394,29 +25394,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="158"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25438,27 +25438,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25480,27 +25480,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="172"/>
+      <c r="AC22" s="173"/>
+      <c r="AD22" s="173"/>
+      <c r="AE22" s="173"/>
+      <c r="AF22" s="173"/>
+      <c r="AG22" s="173"/>
+      <c r="AH22" s="174"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="157" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="158"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25830,68 +25830,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="498ada7362b9f367b0ad53f1b26877d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1476f59a5677fe7b272908915e2ed05" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26126,8 +26064,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26135,5 +26135,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-10-10 17:30:37 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29404"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{A7D92622-B2E5-4E59-B8B9-C627DE387794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2040,24 +2040,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2094,13 +2076,31 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2737,43 +2737,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="163" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-      <c r="AF1" s="163"/>
+      <c r="A1" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="157"/>
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="157"/>
+      <c r="AF1" s="157"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2869,19 +2869,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
-      <c r="AL2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="160"/>
-      <c r="AN2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
+      <c r="AL2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="172"/>
+      <c r="AN2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4231,15 +4231,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4261,29 +4261,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4305,27 +4305,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4347,27 +4347,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4659,6 +4659,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4666,12 +4672,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4687,9 +4687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439DF5C5-7B05-42AC-912E-093F75C23909}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -4744,7 +4744,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4840,14 +4840,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -5553,8 +5553,8 @@
       <c r="Q9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="82" t="s">
-        <v>23</v>
+      <c r="R9" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>17</v>
@@ -5605,11 +5605,11 @@
       </c>
       <c r="AI9" s="1">
         <f t="shared" ref="AI9" si="1">COUNTIF(B9:AF9,"U")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="15" customHeight="1">
@@ -6161,7 +6161,7 @@
       </c>
       <c r="R15" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S15" s="70">
         <f t="shared" si="5"/>
@@ -6223,15 +6223,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6253,29 +6253,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6297,27 +6297,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6339,27 +6339,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6679,7 +6679,7 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AI17" sqref="AI17"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -6734,7 +6734,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6827,14 +6827,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7567,7 +7567,7 @@
       <c r="AF9"/>
       <c r="AG9" s="1">
         <f>'OCT25'!AJ9</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AH9" s="1">
         <f t="shared" si="1"/>
@@ -7575,7 +7575,7 @@
       </c>
       <c r="AI9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15" customHeight="1">
@@ -8171,15 +8171,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8201,29 +8201,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8245,27 +8245,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8287,27 +8287,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8626,9 +8626,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DFC48C-09FC-43B2-ADD0-28180192959C}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AL18" sqref="AL18"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8683,7 +8683,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8779,14 +8779,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="AG9"/>
       <c r="AH9" s="1">
         <f>'NOV25'!AI9</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI9" s="1">
         <f t="shared" ref="AI9:AI11" si="1">COUNTIF(B9:AF9,"U")</f>
@@ -9548,7 +9548,7 @@
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="15" customHeight="1">
@@ -10162,15 +10162,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10192,29 +10192,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10236,27 +10236,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10278,27 +10278,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10641,40 +10641,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
+      <c r="A1" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="176"/>
+      <c r="W1" s="176"/>
+      <c r="X1" s="176"/>
+      <c r="Y1" s="176"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10761,19 +10761,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="160"/>
-      <c r="AG2" s="161"/>
-      <c r="AI2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="160"/>
-      <c r="AK2" s="161"/>
+      <c r="AE2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="173"/>
+      <c r="AI2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -12023,15 +12023,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12053,29 +12053,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12097,27 +12097,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12139,27 +12139,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12451,6 +12451,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12459,11 +12464,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12539,7 +12539,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12635,19 +12635,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
-      <c r="AL2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="160"/>
-      <c r="AN2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
+      <c r="AL2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="172"/>
+      <c r="AN2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -14009,15 +14009,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14051,15 +14051,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14093,15 +14093,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14135,15 +14135,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14521,7 +14521,7 @@
       <c r="AE1" s="178"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14614,19 +14614,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
-      <c r="AK2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="160"/>
-      <c r="AM2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
+      <c r="AK2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="172"/>
+      <c r="AM2" s="173"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15947,15 +15947,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15989,15 +15989,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16031,15 +16031,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16073,15 +16073,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16373,6 +16373,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16380,11 +16385,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16457,7 +16457,7 @@
       <c r="AF1" s="178"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16553,14 +16553,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17831,15 +17831,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17861,29 +17861,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17905,27 +17905,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17947,27 +17947,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18259,18 +18259,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AB19:AH21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18306,42 +18306,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="176" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
+      <c r="A1" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="176"/>
+      <c r="W1" s="176"/>
+      <c r="X1" s="176"/>
+      <c r="Y1" s="176"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="176"/>
+      <c r="AB1" s="176"/>
+      <c r="AC1" s="176"/>
+      <c r="AD1" s="176"/>
+      <c r="AE1" s="176"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18434,14 +18434,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19675,15 +19675,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19710,15 +19710,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19745,15 +19745,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19780,15 +19780,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20164,7 +20164,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20260,14 +20260,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21567,15 +21567,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21602,15 +21602,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21637,15 +21637,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21672,15 +21672,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -21998,7 +21998,7 @@
   <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -22055,7 +22055,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22151,14 +22151,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="161"/>
+      <c r="AH2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23428,15 +23428,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="162" t="s">
+      <c r="F19" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="162"/>
-      <c r="H19" s="162"/>
-      <c r="I19" s="162" t="s">
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="162"/>
+      <c r="J19" s="174"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23458,29 +23458,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="166" t="s">
+      <c r="AB19" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="167"/>
-      <c r="AD19" s="167"/>
-      <c r="AE19" s="167"/>
-      <c r="AF19" s="167"/>
-      <c r="AG19" s="167"/>
-      <c r="AH19" s="168"/>
+      <c r="AC19" s="161"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="162"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="157" t="s">
+      <c r="F20" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158" t="s">
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="158"/>
+      <c r="J20" s="170"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23502,27 +23502,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="169"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AB20" s="163"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23544,27 +23544,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23887,8 +23887,8 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="T17" sqref="T17"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -23942,7 +23942,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="164">
+      <c r="A2" s="158">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -24035,14 +24035,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="159" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="161"/>
+      <c r="AG2" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="173"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="165"/>
+      <c r="A3" s="159"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25364,15 +25364,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="162"/>
-      <c r="H20" s="162"/>
-      <c r="I20" s="162" t="s">
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="162"/>
+      <c r="J20" s="174"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25394,29 +25394,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="166" t="s">
+      <c r="AB20" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="162"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="157" t="s">
+      <c r="F21" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158" t="s">
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="158"/>
+      <c r="J21" s="170"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25438,27 +25438,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="163"/>
+      <c r="AC21" s="164"/>
+      <c r="AD21" s="164"/>
+      <c r="AE21" s="164"/>
+      <c r="AF21" s="164"/>
+      <c r="AG21" s="164"/>
+      <c r="AH21" s="165"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="157" t="s">
+      <c r="F22" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158" t="s">
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="158"/>
+      <c r="J22" s="170"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25480,27 +25480,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="172"/>
-      <c r="AC22" s="173"/>
-      <c r="AD22" s="173"/>
-      <c r="AE22" s="173"/>
-      <c r="AF22" s="173"/>
-      <c r="AG22" s="173"/>
-      <c r="AH22" s="174"/>
+      <c r="AB22" s="166"/>
+      <c r="AC22" s="167"/>
+      <c r="AD22" s="167"/>
+      <c r="AE22" s="167"/>
+      <c r="AF22" s="167"/>
+      <c r="AG22" s="167"/>
+      <c r="AH22" s="168"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="157" t="s">
+      <c r="F23" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="158" t="s">
+      <c r="G23" s="170"/>
+      <c r="H23" s="170"/>
+      <c r="I23" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="158"/>
+      <c r="J23" s="170"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25830,6 +25830,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="498ada7362b9f367b0ad53f1b26877d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1476f59a5677fe7b272908915e2ed05" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26064,70 +26126,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26135,5 +26135,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-10-20 17:31:57 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{A7D92622-B2E5-4E59-B8B9-C627DE387794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -828,7 +828,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1563,24 +1563,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2037,8 +2024,23 @@
     <xf numFmtId="0" fontId="27" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2076,31 +2078,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2737,43 +2721,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="157" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
-      <c r="J1" s="157"/>
-      <c r="K1" s="157"/>
-      <c r="L1" s="157"/>
-      <c r="M1" s="157"/>
-      <c r="N1" s="157"/>
-      <c r="O1" s="157"/>
-      <c r="P1" s="157"/>
-      <c r="Q1" s="157"/>
-      <c r="R1" s="157"/>
-      <c r="S1" s="157"/>
-      <c r="T1" s="157"/>
-      <c r="U1" s="157"/>
-      <c r="V1" s="157"/>
-      <c r="W1" s="157"/>
-      <c r="X1" s="157"/>
-      <c r="Y1" s="157"/>
-      <c r="Z1" s="157"/>
-      <c r="AA1" s="157"/>
-      <c r="AB1" s="157"/>
-      <c r="AC1" s="157"/>
-      <c r="AD1" s="157"/>
-      <c r="AE1" s="157"/>
-      <c r="AF1" s="157"/>
+      <c r="A1" s="162" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
+      <c r="L1" s="162"/>
+      <c r="M1" s="162"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="162"/>
+      <c r="P1" s="162"/>
+      <c r="Q1" s="162"/>
+      <c r="R1" s="162"/>
+      <c r="S1" s="162"/>
+      <c r="T1" s="162"/>
+      <c r="U1" s="162"/>
+      <c r="V1" s="162"/>
+      <c r="W1" s="162"/>
+      <c r="X1" s="162"/>
+      <c r="Y1" s="162"/>
+      <c r="Z1" s="162"/>
+      <c r="AA1" s="162"/>
+      <c r="AB1" s="162"/>
+      <c r="AC1" s="162"/>
+      <c r="AD1" s="162"/>
+      <c r="AE1" s="162"/>
+      <c r="AF1" s="162"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2869,19 +2853,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
-      <c r="AL2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
+      <c r="AL2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="159"/>
+      <c r="AN2" s="160"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4231,15 +4215,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4261,29 +4245,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="166"/>
+      <c r="AD19" s="166"/>
+      <c r="AE19" s="166"/>
+      <c r="AF19" s="166"/>
+      <c r="AG19" s="166"/>
+      <c r="AH19" s="167"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4305,27 +4289,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="168"/>
+      <c r="AC20" s="169"/>
+      <c r="AD20" s="169"/>
+      <c r="AE20" s="169"/>
+      <c r="AF20" s="169"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="170"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4347,27 +4331,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="171"/>
+      <c r="AC21" s="172"/>
+      <c r="AD21" s="172"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="173"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4659,12 +4643,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4672,6 +4650,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4688,7 +4672,7 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -4704,47 +4688,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="182"/>
-      <c r="N1" s="182"/>
-      <c r="O1" s="182"/>
-      <c r="P1" s="182"/>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="182"/>
-      <c r="S1" s="182"/>
-      <c r="T1" s="182"/>
-      <c r="U1" s="182"/>
-      <c r="V1" s="182"/>
-      <c r="W1" s="182"/>
-      <c r="X1" s="182"/>
-      <c r="Y1" s="182"/>
-      <c r="Z1" s="182"/>
-      <c r="AA1" s="182"/>
-      <c r="AB1" s="182"/>
-      <c r="AC1" s="182"/>
-      <c r="AD1" s="182"/>
-      <c r="AE1" s="182"/>
-      <c r="AF1" s="182"/>
+      <c r="A1" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4840,14 +4824,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="174"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6223,15 +6207,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6253,29 +6237,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="166"/>
+      <c r="AD20" s="166"/>
+      <c r="AE20" s="166"/>
+      <c r="AF20" s="166"/>
+      <c r="AG20" s="166"/>
+      <c r="AH20" s="167"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6297,27 +6281,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="168"/>
+      <c r="AC21" s="169"/>
+      <c r="AD21" s="169"/>
+      <c r="AE21" s="169"/>
+      <c r="AF21" s="169"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="170"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6339,27 +6323,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="171"/>
+      <c r="AC22" s="172"/>
+      <c r="AD22" s="172"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="173"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6679,8 +6663,8 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AI17" sqref="AI17"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -6695,46 +6679,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="183" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="184"/>
-      <c r="S1" s="184"/>
-      <c r="T1" s="184"/>
-      <c r="U1" s="184"/>
-      <c r="V1" s="184"/>
-      <c r="W1" s="184"/>
-      <c r="X1" s="184"/>
-      <c r="Y1" s="184"/>
-      <c r="Z1" s="184"/>
-      <c r="AA1" s="184"/>
-      <c r="AB1" s="184"/>
-      <c r="AC1" s="184"/>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
+      <c r="G1" s="183"/>
+      <c r="H1" s="183"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="183"/>
+      <c r="K1" s="183"/>
+      <c r="L1" s="183"/>
+      <c r="M1" s="183"/>
+      <c r="N1" s="183"/>
+      <c r="O1" s="183"/>
+      <c r="P1" s="183"/>
+      <c r="Q1" s="183"/>
+      <c r="R1" s="183"/>
+      <c r="S1" s="183"/>
+      <c r="T1" s="183"/>
+      <c r="U1" s="183"/>
+      <c r="V1" s="183"/>
+      <c r="W1" s="183"/>
+      <c r="X1" s="183"/>
+      <c r="Y1" s="183"/>
+      <c r="Z1" s="183"/>
+      <c r="AA1" s="183"/>
+      <c r="AB1" s="183"/>
+      <c r="AC1" s="183"/>
+      <c r="AD1" s="183"/>
+      <c r="AE1" s="183"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6827,14 +6811,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="160"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7370,14 +7354,14 @@
       <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="83" t="s">
-        <v>26</v>
+      <c r="C8" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="82" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>17</v>
@@ -7385,11 +7369,11 @@
       <c r="G8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="156" t="s">
-        <v>26</v>
+      <c r="H8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="81" t="s">
+        <v>21</v>
       </c>
       <c r="J8" s="83" t="s">
         <v>26</v>
@@ -7424,20 +7408,20 @@
       <c r="T8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U8" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="V8" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="W8" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="X8" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y8" s="81" t="s">
-        <v>21</v>
+      <c r="U8" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="Z8" s="123" t="s">
         <v>17</v>
@@ -7948,11 +7932,11 @@
       </c>
       <c r="H14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="70">
         <f t="shared" si="5"/>
@@ -8000,23 +7984,23 @@
       </c>
       <c r="U14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="70">
         <f t="shared" si="5"/>
@@ -8053,15 +8037,15 @@
       </c>
       <c r="C15" s="70">
         <f t="shared" ref="C15:AE15" si="6">COUNTIF(C2:C11,"P14")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="70">
         <f t="shared" si="6"/>
@@ -8171,15 +8155,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8201,29 +8185,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="166"/>
+      <c r="AD20" s="166"/>
+      <c r="AE20" s="166"/>
+      <c r="AF20" s="166"/>
+      <c r="AG20" s="166"/>
+      <c r="AH20" s="167"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8245,27 +8229,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="168"/>
+      <c r="AC21" s="169"/>
+      <c r="AD21" s="169"/>
+      <c r="AE21" s="169"/>
+      <c r="AF21" s="169"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="170"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8287,27 +8271,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="171"/>
+      <c r="AC22" s="172"/>
+      <c r="AD22" s="172"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="173"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8627,8 +8611,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AL18" sqref="AL18"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10:P10"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8643,47 +8627,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="185" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="187"/>
-      <c r="M1" s="187"/>
-      <c r="N1" s="187"/>
-      <c r="O1" s="187"/>
-      <c r="P1" s="187"/>
-      <c r="Q1" s="188"/>
-      <c r="R1" s="188"/>
-      <c r="S1" s="187"/>
-      <c r="T1" s="187"/>
-      <c r="U1" s="187"/>
-      <c r="V1" s="187"/>
-      <c r="W1" s="187"/>
-      <c r="X1" s="188"/>
-      <c r="Y1" s="188"/>
-      <c r="Z1" s="187"/>
-      <c r="AA1" s="187"/>
-      <c r="AB1" s="187"/>
-      <c r="AC1" s="187"/>
-      <c r="AD1" s="187"/>
-      <c r="AE1" s="188"/>
-      <c r="AF1" s="189"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+      <c r="N1" s="186"/>
+      <c r="O1" s="186"/>
+      <c r="P1" s="186"/>
+      <c r="Q1" s="187"/>
+      <c r="R1" s="187"/>
+      <c r="S1" s="186"/>
+      <c r="T1" s="186"/>
+      <c r="U1" s="186"/>
+      <c r="V1" s="186"/>
+      <c r="W1" s="186"/>
+      <c r="X1" s="187"/>
+      <c r="Y1" s="187"/>
+      <c r="Z1" s="186"/>
+      <c r="AA1" s="186"/>
+      <c r="AB1" s="186"/>
+      <c r="AC1" s="186"/>
+      <c r="AD1" s="186"/>
+      <c r="AE1" s="187"/>
+      <c r="AF1" s="188"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8779,14 +8763,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="174"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -8903,11 +8887,11 @@
       <c r="D4" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>16</v>
+      <c r="E4" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
@@ -8993,11 +8977,11 @@
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -10162,15 +10146,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10192,29 +10176,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="166"/>
+      <c r="AD20" s="166"/>
+      <c r="AE20" s="166"/>
+      <c r="AF20" s="166"/>
+      <c r="AG20" s="166"/>
+      <c r="AH20" s="167"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10236,27 +10220,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="168"/>
+      <c r="AC21" s="169"/>
+      <c r="AD21" s="169"/>
+      <c r="AE21" s="169"/>
+      <c r="AF21" s="169"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="170"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10278,27 +10262,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="171"/>
+      <c r="AC22" s="172"/>
+      <c r="AD22" s="172"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="173"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10674,7 +10658,7 @@
       <c r="AC1" s="175"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10761,19 +10745,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="173"/>
-      <c r="AI2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="173"/>
+      <c r="AE2" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="159"/>
+      <c r="AG2" s="160"/>
+      <c r="AI2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="160"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="174"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -12023,15 +12007,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12053,29 +12037,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="166"/>
+      <c r="AD19" s="166"/>
+      <c r="AE19" s="166"/>
+      <c r="AF19" s="166"/>
+      <c r="AG19" s="166"/>
+      <c r="AH19" s="167"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12097,27 +12081,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="168"/>
+      <c r="AC20" s="169"/>
+      <c r="AD20" s="169"/>
+      <c r="AE20" s="169"/>
+      <c r="AF20" s="169"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="170"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12139,27 +12123,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="171"/>
+      <c r="AC21" s="172"/>
+      <c r="AD21" s="172"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="173"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12451,11 +12435,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12464,6 +12443,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12503,43 +12487,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
+      <c r="A1" s="177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12635,19 +12619,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
-      <c r="AL2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
+      <c r="AL2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="159"/>
+      <c r="AN2" s="160"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -14009,15 +13993,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14051,15 +14035,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14093,15 +14077,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14135,15 +14119,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14486,42 +14470,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
+      <c r="A1" s="177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14614,19 +14598,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
-      <c r="AK2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="172"/>
-      <c r="AM2" s="173"/>
+      <c r="AG2" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="160"/>
+      <c r="AK2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="159"/>
+      <c r="AM2" s="160"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15947,15 +15931,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15989,15 +15973,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16031,15 +16015,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16073,15 +16057,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16373,11 +16357,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16385,6 +16364,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16421,43 +16405,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
+      <c r="A1" s="177" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16553,14 +16537,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17831,15 +17815,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17861,29 +17845,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="166"/>
+      <c r="AD19" s="166"/>
+      <c r="AE19" s="166"/>
+      <c r="AF19" s="166"/>
+      <c r="AG19" s="166"/>
+      <c r="AH19" s="167"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17905,27 +17889,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="168"/>
+      <c r="AC20" s="169"/>
+      <c r="AD20" s="169"/>
+      <c r="AE20" s="169"/>
+      <c r="AF20" s="169"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="170"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17947,27 +17931,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="171"/>
+      <c r="AC21" s="172"/>
+      <c r="AD21" s="172"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="173"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18259,18 +18243,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18341,7 +18325,7 @@
       <c r="AE1" s="176"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18434,14 +18418,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="160"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19675,15 +19659,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19710,15 +19694,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19745,15 +19729,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19780,15 +19764,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20164,7 +20148,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20260,14 +20244,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -20631,25 +20615,25 @@
       <c r="M6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="179"/>
-      <c r="O6" s="180"/>
-      <c r="P6" s="180"/>
-      <c r="Q6" s="180"/>
-      <c r="R6" s="180"/>
-      <c r="S6" s="180"/>
-      <c r="T6" s="180"/>
-      <c r="U6" s="180"/>
-      <c r="V6" s="180"/>
-      <c r="W6" s="180"/>
-      <c r="X6" s="180"/>
-      <c r="Y6" s="180"/>
-      <c r="Z6" s="180"/>
-      <c r="AA6" s="180"/>
-      <c r="AB6" s="180"/>
-      <c r="AC6" s="180"/>
-      <c r="AD6" s="180"/>
-      <c r="AE6" s="180"/>
-      <c r="AF6" s="181"/>
+      <c r="N6" s="178"/>
+      <c r="O6" s="179"/>
+      <c r="P6" s="179"/>
+      <c r="Q6" s="179"/>
+      <c r="R6" s="179"/>
+      <c r="S6" s="179"/>
+      <c r="T6" s="179"/>
+      <c r="U6" s="179"/>
+      <c r="V6" s="179"/>
+      <c r="W6" s="179"/>
+      <c r="X6" s="179"/>
+      <c r="Y6" s="179"/>
+      <c r="Z6" s="179"/>
+      <c r="AA6" s="179"/>
+      <c r="AB6" s="179"/>
+      <c r="AC6" s="179"/>
+      <c r="AD6" s="179"/>
+      <c r="AE6" s="179"/>
+      <c r="AF6" s="180"/>
       <c r="AG6"/>
       <c r="AH6" s="1">
         <f>'JUN25'!AI6</f>
@@ -21567,15 +21551,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21602,15 +21586,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21637,15 +21621,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21672,15 +21656,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22015,47 +21999,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
-      <c r="K1" s="183"/>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="183"/>
-      <c r="R1" s="183"/>
-      <c r="S1" s="183"/>
-      <c r="T1" s="183"/>
-      <c r="U1" s="183"/>
-      <c r="V1" s="183"/>
-      <c r="W1" s="183"/>
-      <c r="X1" s="183"/>
-      <c r="Y1" s="183"/>
-      <c r="Z1" s="183"/>
-      <c r="AA1" s="183"/>
-      <c r="AB1" s="183"/>
-      <c r="AC1" s="183"/>
-      <c r="AD1" s="183"/>
-      <c r="AE1" s="183"/>
-      <c r="AF1" s="183"/>
+      <c r="A1" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="182"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="182"/>
+      <c r="N1" s="182"/>
+      <c r="O1" s="182"/>
+      <c r="P1" s="182"/>
+      <c r="Q1" s="182"/>
+      <c r="R1" s="182"/>
+      <c r="S1" s="182"/>
+      <c r="T1" s="182"/>
+      <c r="U1" s="182"/>
+      <c r="V1" s="182"/>
+      <c r="W1" s="182"/>
+      <c r="X1" s="182"/>
+      <c r="Y1" s="182"/>
+      <c r="Z1" s="182"/>
+      <c r="AA1" s="182"/>
+      <c r="AB1" s="182"/>
+      <c r="AC1" s="182"/>
+      <c r="AD1" s="182"/>
+      <c r="AE1" s="182"/>
+      <c r="AF1" s="182"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22151,14 +22135,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
+      <c r="AH2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="160"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="177"/>
+      <c r="A3" s="174"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23428,15 +23412,15 @@
     <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="174" t="s">
+      <c r="F19" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174" t="s">
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="174"/>
+      <c r="J19" s="161"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23458,29 +23442,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="160" t="s">
+      <c r="AB19" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="161"/>
-      <c r="AD19" s="161"/>
-      <c r="AE19" s="161"/>
-      <c r="AF19" s="161"/>
-      <c r="AG19" s="161"/>
-      <c r="AH19" s="162"/>
+      <c r="AC19" s="166"/>
+      <c r="AD19" s="166"/>
+      <c r="AE19" s="166"/>
+      <c r="AF19" s="166"/>
+      <c r="AG19" s="166"/>
+      <c r="AH19" s="167"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="169" t="s">
+      <c r="F20" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="170"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23502,27 +23486,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="163"/>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AB20" s="168"/>
+      <c r="AC20" s="169"/>
+      <c r="AD20" s="169"/>
+      <c r="AE20" s="169"/>
+      <c r="AF20" s="169"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="170"/>
     </row>
     <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23544,27 +23528,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="171"/>
+      <c r="AC21" s="172"/>
+      <c r="AD21" s="172"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="173"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23903,46 +23887,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="184" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
-      <c r="M1" s="185"/>
-      <c r="N1" s="185"/>
-      <c r="O1" s="185"/>
-      <c r="P1" s="185"/>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="185"/>
-      <c r="S1" s="185"/>
-      <c r="T1" s="185"/>
-      <c r="U1" s="185"/>
-      <c r="V1" s="185"/>
-      <c r="W1" s="185"/>
-      <c r="X1" s="185"/>
-      <c r="Y1" s="185"/>
-      <c r="Z1" s="185"/>
-      <c r="AA1" s="185"/>
-      <c r="AB1" s="185"/>
-      <c r="AC1" s="185"/>
-      <c r="AD1" s="185"/>
-      <c r="AE1" s="185"/>
+      <c r="A1" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
+      <c r="J1" s="184"/>
+      <c r="K1" s="184"/>
+      <c r="L1" s="184"/>
+      <c r="M1" s="184"/>
+      <c r="N1" s="184"/>
+      <c r="O1" s="184"/>
+      <c r="P1" s="184"/>
+      <c r="Q1" s="184"/>
+      <c r="R1" s="184"/>
+      <c r="S1" s="184"/>
+      <c r="T1" s="184"/>
+      <c r="U1" s="184"/>
+      <c r="V1" s="184"/>
+      <c r="W1" s="184"/>
+      <c r="X1" s="184"/>
+      <c r="Y1" s="184"/>
+      <c r="Z1" s="184"/>
+      <c r="AA1" s="184"/>
+      <c r="AB1" s="184"/>
+      <c r="AC1" s="184"/>
+      <c r="AD1" s="184"/>
+      <c r="AE1" s="184"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="158">
+      <c r="A2" s="163">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -24035,14 +24019,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="173"/>
+      <c r="AG2" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="160"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="159"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25364,15 +25348,15 @@
     <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="174" t="s">
+      <c r="F20" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="174"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25394,29 +25378,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="160" t="s">
+      <c r="AB20" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="161"/>
-      <c r="AD20" s="161"/>
-      <c r="AE20" s="161"/>
-      <c r="AF20" s="161"/>
-      <c r="AG20" s="161"/>
-      <c r="AH20" s="162"/>
+      <c r="AC20" s="166"/>
+      <c r="AD20" s="166"/>
+      <c r="AE20" s="166"/>
+      <c r="AF20" s="166"/>
+      <c r="AG20" s="166"/>
+      <c r="AH20" s="167"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="169" t="s">
+      <c r="F21" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="170"/>
-      <c r="H21" s="170"/>
-      <c r="I21" s="170" t="s">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="170"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25438,27 +25422,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="163"/>
-      <c r="AC21" s="164"/>
-      <c r="AD21" s="164"/>
-      <c r="AE21" s="164"/>
-      <c r="AF21" s="164"/>
-      <c r="AG21" s="164"/>
-      <c r="AH21" s="165"/>
+      <c r="AB21" s="168"/>
+      <c r="AC21" s="169"/>
+      <c r="AD21" s="169"/>
+      <c r="AE21" s="169"/>
+      <c r="AF21" s="169"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="170"/>
     </row>
     <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="169" t="s">
+      <c r="F22" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="170"/>
-      <c r="H22" s="170"/>
-      <c r="I22" s="170" t="s">
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="170"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25480,27 +25464,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="167"/>
-      <c r="AD22" s="167"/>
-      <c r="AE22" s="167"/>
-      <c r="AF22" s="167"/>
-      <c r="AG22" s="167"/>
-      <c r="AH22" s="168"/>
+      <c r="AB22" s="171"/>
+      <c r="AC22" s="172"/>
+      <c r="AD22" s="172"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="173"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="169" t="s">
+      <c r="F23" s="156" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="170"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="170" t="s">
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="170"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25839,61 +25823,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="498ada7362b9f367b0ad53f1b26877d8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1476f59a5677fe7b272908915e2ed05" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6ee96d7c0753969b9e06c1757a47325">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a2ac023326aa581855272ff7514c98af" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
     <xsd:import namespace="fa453329-a4c9-4120-b786-6a0f9fa17d90"/>
     <xsd:element name="properties">
@@ -25916,6 +25847,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -25983,6 +25915,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -26126,14 +26063,67 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F192D2-FE2D-40B9-B3AF-4CBE16686856}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC8886C-FC11-4759-832F-4320E06624ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-10-31 21:46:27 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2234,6 +2234,24 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2270,31 +2288,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2333,33 +2333,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2379,6 +2352,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3013,43 +3013,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
-      <c r="V1" s="201"/>
-      <c r="W1" s="201"/>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="201"/>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="201"/>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="201"/>
-      <c r="AD1" s="201"/>
-      <c r="AE1" s="201"/>
-      <c r="AF1" s="201"/>
+      <c r="A1" s="207" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="207"/>
+      <c r="I1" s="207"/>
+      <c r="J1" s="207"/>
+      <c r="K1" s="207"/>
+      <c r="L1" s="207"/>
+      <c r="M1" s="207"/>
+      <c r="N1" s="207"/>
+      <c r="O1" s="207"/>
+      <c r="P1" s="207"/>
+      <c r="Q1" s="207"/>
+      <c r="R1" s="207"/>
+      <c r="S1" s="207"/>
+      <c r="T1" s="207"/>
+      <c r="U1" s="207"/>
+      <c r="V1" s="207"/>
+      <c r="W1" s="207"/>
+      <c r="X1" s="207"/>
+      <c r="Y1" s="207"/>
+      <c r="Z1" s="207"/>
+      <c r="AA1" s="207"/>
+      <c r="AB1" s="207"/>
+      <c r="AC1" s="207"/>
+      <c r="AD1" s="207"/>
+      <c r="AE1" s="207"/>
+      <c r="AF1" s="207"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -3145,19 +3145,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
-      <c r="AL2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
+      <c r="AL2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="204"/>
+      <c r="AN2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4507,15 +4507,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4537,29 +4537,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4581,27 +4581,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4623,27 +4623,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4935,12 +4935,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4948,6 +4942,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
@@ -4964,8 +4964,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AJ15" sqref="AJ15"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -5020,7 +5020,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -5116,14 +5116,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -5232,10 +5232,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" s="83" t="s">
         <v>26</v>
@@ -5247,19 +5247,19 @@
         <v>17</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>17</v>
@@ -5268,19 +5268,19 @@
         <v>17</v>
       </c>
       <c r="N4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>17</v>
@@ -5289,19 +5289,19 @@
         <v>17</v>
       </c>
       <c r="U4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="V4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="W4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>71</v>
       </c>
       <c r="Y4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>17</v>
@@ -5310,19 +5310,19 @@
         <v>17</v>
       </c>
       <c r="AB4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AC4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AD4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AE4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AF4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AH4" s="1">
         <f>'SEP25'!AI4</f>
@@ -6499,15 +6499,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6529,29 +6529,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6573,27 +6573,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6615,27 +6615,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6955,8 +6955,8 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Z17" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -7010,7 +7010,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -7103,14 +7103,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7222,19 +7222,19 @@
         <v>17</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>17</v>
@@ -7243,19 +7243,19 @@
         <v>17</v>
       </c>
       <c r="K4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="M4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>17</v>
@@ -8447,15 +8447,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8477,29 +8477,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8521,27 +8521,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8563,27 +8563,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8903,8 +8903,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AM28" sqref="AM28"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8959,7 +8959,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -9055,14 +9055,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9195,16 +9195,16 @@
         <v>15</v>
       </c>
       <c r="J4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="M4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>17</v>
@@ -9213,19 +9213,19 @@
         <v>17</v>
       </c>
       <c r="P4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="S4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>17</v>
@@ -9234,13 +9234,13 @@
         <v>17</v>
       </c>
       <c r="W4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="X4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Y4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Z4" s="157" t="s">
         <v>15</v>
@@ -9255,13 +9255,13 @@
         <v>17</v>
       </c>
       <c r="AD4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AE4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AF4" s="72" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AH4" s="1">
         <f>'NOV25'!AI4</f>
@@ -10438,15 +10438,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10468,29 +10468,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10512,27 +10512,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10554,27 +10554,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10894,7 +10894,7 @@
   <dimension ref="A1:AN30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL18" sqref="AL18"/>
+      <selection activeCell="AA4" sqref="AA4:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.95"/>
@@ -10905,40 +10905,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="243" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="243"/>
-      <c r="J1" s="243"/>
-      <c r="K1" s="243"/>
-      <c r="L1" s="243"/>
-      <c r="M1" s="243"/>
-      <c r="N1" s="243"/>
-      <c r="O1" s="243"/>
-      <c r="P1" s="243"/>
-      <c r="Q1" s="243"/>
-      <c r="R1" s="243"/>
-      <c r="S1" s="243"/>
-      <c r="T1" s="243"/>
-      <c r="U1" s="243"/>
-      <c r="V1" s="243"/>
-      <c r="W1" s="243"/>
-      <c r="X1" s="243"/>
-      <c r="Y1" s="243"/>
-      <c r="Z1" s="243"/>
-      <c r="AA1" s="243"/>
-      <c r="AB1" s="243"/>
-      <c r="AC1" s="243"/>
-      <c r="AD1" s="243"/>
-      <c r="AE1" s="243"/>
-      <c r="AF1" s="243"/>
+      <c r="A1" s="234" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="234"/>
+      <c r="C1" s="234"/>
+      <c r="D1" s="234"/>
+      <c r="E1" s="234"/>
+      <c r="F1" s="234"/>
+      <c r="G1" s="234"/>
+      <c r="H1" s="234"/>
+      <c r="I1" s="234"/>
+      <c r="J1" s="234"/>
+      <c r="K1" s="234"/>
+      <c r="L1" s="234"/>
+      <c r="M1" s="234"/>
+      <c r="N1" s="234"/>
+      <c r="O1" s="234"/>
+      <c r="P1" s="234"/>
+      <c r="Q1" s="234"/>
+      <c r="R1" s="234"/>
+      <c r="S1" s="234"/>
+      <c r="T1" s="234"/>
+      <c r="U1" s="234"/>
+      <c r="V1" s="234"/>
+      <c r="W1" s="234"/>
+      <c r="X1" s="234"/>
+      <c r="Y1" s="234"/>
+      <c r="Z1" s="234"/>
+      <c r="AA1" s="234"/>
+      <c r="AB1" s="234"/>
+      <c r="AC1" s="234"/>
+      <c r="AD1" s="234"/>
+      <c r="AE1" s="234"/>
+      <c r="AF1" s="234"/>
       <c r="AG1" s="159"/>
       <c r="AH1" s="159"/>
       <c r="AI1" s="159"/>
@@ -10949,7 +10949,7 @@
       <c r="AN1" s="159"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="244">
+      <c r="A2" s="235">
         <v>46023</v>
       </c>
       <c r="B2" s="161">
@@ -11076,19 +11076,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="245" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="246"/>
-      <c r="AJ2" s="246"/>
-      <c r="AL2" s="245" t="s">
+      <c r="AH2" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="237"/>
+      <c r="AJ2" s="237"/>
+      <c r="AL2" s="236" t="s">
         <v>103</v>
       </c>
-      <c r="AM2" s="246"/>
-      <c r="AN2" s="246"/>
+      <c r="AM2" s="237"/>
+      <c r="AN2" s="237"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="244"/>
+      <c r="A3" s="235"/>
       <c r="B3" s="161" t="str">
         <f t="shared" ref="B3:AF3" si="1">UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -11240,7 +11240,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" s="167" t="s">
         <v>17</v>
@@ -11249,19 +11249,19 @@
         <v>17</v>
       </c>
       <c r="F4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" s="167" t="s">
         <v>17</v>
@@ -11270,19 +11270,19 @@
         <v>17</v>
       </c>
       <c r="M4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R4" s="167" t="s">
         <v>17</v>
@@ -11291,19 +11291,19 @@
         <v>17</v>
       </c>
       <c r="T4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="U4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="V4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="W4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="X4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Y4" s="167" t="s">
         <v>17</v>
@@ -11312,19 +11312,19 @@
         <v>17</v>
       </c>
       <c r="AA4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AB4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AC4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AD4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AE4" s="166" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AF4" s="167" t="s">
         <v>17</v>
@@ -11479,8 +11479,8 @@
       <c r="B6" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="170" t="s">
-        <v>68</v>
+      <c r="C6" s="166" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="167" t="s">
         <v>17</v>
@@ -12454,14 +12454,14 @@
     </row>
     <row r="16" spans="1:40">
       <c r="E16" s="174"/>
-      <c r="F16" s="247" t="s">
+      <c r="F16" s="238" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="248"/>
-      <c r="H16" s="247" t="s">
+      <c r="G16" s="239"/>
+      <c r="H16" s="238" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="249"/>
+      <c r="I16" s="240"/>
       <c r="M16" s="168" t="s">
         <v>17</v>
       </c>
@@ -12487,14 +12487,14 @@
       <c r="E17" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="240" t="s">
+      <c r="F17" s="241" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="241"/>
-      <c r="H17" s="240" t="s">
+      <c r="G17" s="242"/>
+      <c r="H17" s="241" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="242"/>
+      <c r="I17" s="243"/>
       <c r="M17" s="181" t="s">
         <v>42</v>
       </c>
@@ -12520,14 +12520,14 @@
       <c r="E18" s="166" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="234" t="s">
+      <c r="F18" s="244" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="235"/>
-      <c r="H18" s="234" t="s">
+      <c r="G18" s="245"/>
+      <c r="H18" s="244" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="236"/>
+      <c r="I18" s="246"/>
       <c r="M18" s="161" t="s">
         <v>15</v>
       </c>
@@ -12553,14 +12553,14 @@
       <c r="E19" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="234" t="s">
+      <c r="F19" s="244" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="235"/>
-      <c r="H19" s="234" t="s">
+      <c r="G19" s="245"/>
+      <c r="H19" s="244" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="236"/>
+      <c r="I19" s="246"/>
       <c r="M19" s="187" t="s">
         <v>26</v>
       </c>
@@ -12581,28 +12581,28 @@
       <c r="V19" s="183"/>
       <c r="W19" s="183"/>
       <c r="X19" s="184"/>
-      <c r="AD19" s="204" t="s">
+      <c r="AD19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="205"/>
-      <c r="AI19" s="205"/>
-      <c r="AJ19" s="206"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="211"/>
+      <c r="AI19" s="211"/>
+      <c r="AJ19" s="212"/>
     </row>
     <row r="20" spans="5:36">
       <c r="E20" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="234" t="s">
+      <c r="F20" s="244" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="235"/>
-      <c r="H20" s="234" t="s">
+      <c r="G20" s="245"/>
+      <c r="H20" s="244" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="236"/>
+      <c r="I20" s="246"/>
       <c r="M20" s="187" t="s">
         <v>18</v>
       </c>
@@ -12623,26 +12623,26 @@
       <c r="V20" s="183"/>
       <c r="W20" s="183"/>
       <c r="X20" s="184"/>
-      <c r="AD20" s="207"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="208"/>
-      <c r="AI20" s="208"/>
-      <c r="AJ20" s="209"/>
+      <c r="AD20" s="213"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="214"/>
+      <c r="AI20" s="214"/>
+      <c r="AJ20" s="215"/>
     </row>
     <row r="21" spans="5:36" ht="13.5" thickBot="1">
       <c r="E21" s="188" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="237" t="s">
+      <c r="F21" s="247" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="238"/>
-      <c r="H21" s="237" t="s">
+      <c r="G21" s="248"/>
+      <c r="H21" s="247" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="239"/>
+      <c r="I21" s="249"/>
       <c r="M21" s="189" t="s">
         <v>15</v>
       </c>
@@ -12663,13 +12663,13 @@
       <c r="V21" s="183"/>
       <c r="W21" s="183"/>
       <c r="X21" s="184"/>
-      <c r="AD21" s="210"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="211"/>
-      <c r="AI21" s="211"/>
-      <c r="AJ21" s="212"/>
+      <c r="AD21" s="216"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="217"/>
+      <c r="AI21" s="217"/>
+      <c r="AJ21" s="218"/>
     </row>
     <row r="22" spans="5:36">
       <c r="M22" s="189" t="s">
@@ -12871,23 +12871,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="AD19:AJ21"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AL2:AN2"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="AD19:AJ21"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -12935,40 +12935,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
-      <c r="T1" s="220"/>
-      <c r="U1" s="220"/>
-      <c r="V1" s="220"/>
-      <c r="W1" s="220"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="219"/>
-      <c r="AB1" s="219"/>
-      <c r="AC1" s="219"/>
+      <c r="A1" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="220"/>
+      <c r="AB1" s="220"/>
+      <c r="AC1" s="220"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -13055,19 +13055,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="216"/>
-      <c r="AG2" s="217"/>
-      <c r="AI2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="216"/>
-      <c r="AK2" s="217"/>
+      <c r="AE2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="204"/>
+      <c r="AG2" s="205"/>
+      <c r="AI2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="204"/>
+      <c r="AK2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -14317,15 +14317,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14347,29 +14347,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14391,27 +14391,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14433,27 +14433,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14745,11 +14745,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -14758,6 +14753,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
@@ -14833,7 +14833,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -14929,19 +14929,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
-      <c r="AL2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
+      <c r="AL2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="204"/>
+      <c r="AN2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -16303,15 +16303,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -16345,15 +16345,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16387,15 +16387,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16429,15 +16429,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16815,7 +16815,7 @@
       <c r="AE1" s="222"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -16908,19 +16908,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
-      <c r="AK2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="216"/>
-      <c r="AM2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
+      <c r="AK2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="204"/>
+      <c r="AM2" s="205"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -18241,15 +18241,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -18283,15 +18283,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -18325,15 +18325,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -18367,15 +18367,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18667,11 +18667,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -18679,6 +18674,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -18751,7 +18751,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -18847,14 +18847,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -20125,15 +20125,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -20155,29 +20155,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -20199,27 +20199,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -20241,27 +20241,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20553,18 +20553,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -20600,42 +20600,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
-      <c r="T1" s="220"/>
-      <c r="U1" s="220"/>
-      <c r="V1" s="220"/>
-      <c r="W1" s="220"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="220"/>
-      <c r="AB1" s="220"/>
-      <c r="AC1" s="220"/>
-      <c r="AD1" s="220"/>
-      <c r="AE1" s="220"/>
+      <c r="A1" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="221"/>
+      <c r="AB1" s="221"/>
+      <c r="AC1" s="221"/>
+      <c r="AD1" s="221"/>
+      <c r="AE1" s="221"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -20728,14 +20728,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -21969,15 +21969,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -22004,15 +22004,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -22039,15 +22039,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -22074,15 +22074,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -22458,7 +22458,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -22554,14 +22554,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -23861,15 +23861,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -23896,15 +23896,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -23931,15 +23931,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -23966,15 +23966,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -24349,7 +24349,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -24445,14 +24445,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -25722,15 +25722,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -25752,29 +25752,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -25796,27 +25796,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -25838,27 +25838,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -26236,7 +26236,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -26329,14 +26329,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -27657,15 +27657,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -27687,29 +27687,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -27731,27 +27731,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -27773,27 +27773,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -28364,15 +28364,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
@@ -28425,14 +28416,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-11-04 18:42:42 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="12" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4487" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4485" uniqueCount="106">
   <si>
     <t>LGSP - Lufthansa Ground Services Portugal              NIF : 509 842 593          Atividade: CAE 52230.R3           Sede e local de trabalho: Avenida da Boavista ED.Burgo, 1837 sala 13.4/  Horario de Funcionamento: 24/7   IRT : Nao Aplicavel</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>LGSP - Lufthansa Ground Services Portugal              NIF : 509 842 593          Atividade: CAE 52230.R3           Sede e local de trabalho: Avenida da BoaviP09/a ED.Burgo, 1837 sala 13.4/  Horario de Funcionamento: 24/7   IRT : Nao Aplicavel</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
   <si>
     <t>Ferias 2026</t>
@@ -2234,24 +2237,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2288,13 +2273,31 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2333,6 +2336,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2352,33 +2382,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3013,43 +3016,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="207" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
-      <c r="N1" s="207"/>
-      <c r="O1" s="207"/>
-      <c r="P1" s="207"/>
-      <c r="Q1" s="207"/>
-      <c r="R1" s="207"/>
-      <c r="S1" s="207"/>
-      <c r="T1" s="207"/>
-      <c r="U1" s="207"/>
-      <c r="V1" s="207"/>
-      <c r="W1" s="207"/>
-      <c r="X1" s="207"/>
-      <c r="Y1" s="207"/>
-      <c r="Z1" s="207"/>
-      <c r="AA1" s="207"/>
-      <c r="AB1" s="207"/>
-      <c r="AC1" s="207"/>
-      <c r="AD1" s="207"/>
-      <c r="AE1" s="207"/>
-      <c r="AF1" s="207"/>
+      <c r="A1" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
+      <c r="V1" s="201"/>
+      <c r="W1" s="201"/>
+      <c r="X1" s="201"/>
+      <c r="Y1" s="201"/>
+      <c r="Z1" s="201"/>
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="201"/>
+      <c r="AD1" s="201"/>
+      <c r="AE1" s="201"/>
+      <c r="AF1" s="201"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -3145,19 +3148,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
-      <c r="AL2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="204"/>
-      <c r="AN2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
+      <c r="AL2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="216"/>
+      <c r="AN2" s="217"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4507,15 +4510,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4537,29 +4540,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="210" t="s">
+      <c r="AB19" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="211"/>
-      <c r="AD19" s="211"/>
-      <c r="AE19" s="211"/>
-      <c r="AF19" s="211"/>
-      <c r="AG19" s="211"/>
-      <c r="AH19" s="212"/>
+      <c r="AC19" s="205"/>
+      <c r="AD19" s="205"/>
+      <c r="AE19" s="205"/>
+      <c r="AF19" s="205"/>
+      <c r="AG19" s="205"/>
+      <c r="AH19" s="206"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4581,27 +4584,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="213"/>
-      <c r="AC20" s="214"/>
-      <c r="AD20" s="214"/>
-      <c r="AE20" s="214"/>
-      <c r="AF20" s="214"/>
-      <c r="AG20" s="214"/>
-      <c r="AH20" s="215"/>
+      <c r="AB20" s="207"/>
+      <c r="AC20" s="208"/>
+      <c r="AD20" s="208"/>
+      <c r="AE20" s="208"/>
+      <c r="AF20" s="208"/>
+      <c r="AG20" s="208"/>
+      <c r="AH20" s="209"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4623,27 +4626,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="216"/>
-      <c r="AC21" s="217"/>
-      <c r="AD21" s="217"/>
-      <c r="AE21" s="217"/>
-      <c r="AF21" s="217"/>
-      <c r="AG21" s="217"/>
-      <c r="AH21" s="218"/>
+      <c r="AB21" s="210"/>
+      <c r="AC21" s="211"/>
+      <c r="AD21" s="211"/>
+      <c r="AE21" s="211"/>
+      <c r="AF21" s="211"/>
+      <c r="AG21" s="211"/>
+      <c r="AH21" s="212"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4935,6 +4938,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4942,12 +4951,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
@@ -4964,8 +4967,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AJ15" sqref="AJ15"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AC26" sqref="AC26"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -5020,7 +5023,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -5116,14 +5119,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="219"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6496,18 +6499,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:34" ht="15" thickBot="1"/>
-    <row r="20" spans="5:34">
+    <row r="19" spans="5:25" ht="15"/>
+    <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="206" t="s">
+      <c r="F20" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206" t="s">
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="206"/>
+      <c r="J20" s="218"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6529,29 +6532,20 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="210" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC20" s="211"/>
-      <c r="AD20" s="211"/>
-      <c r="AE20" s="211"/>
-      <c r="AF20" s="211"/>
-      <c r="AG20" s="211"/>
-      <c r="AH20" s="212"/>
-    </row>
-    <row r="21" spans="5:34">
+    </row>
+    <row r="21" spans="5:25" ht="14.45" customHeight="1">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6573,27 +6567,20 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="213"/>
-      <c r="AC21" s="214"/>
-      <c r="AD21" s="214"/>
-      <c r="AE21" s="214"/>
-      <c r="AF21" s="214"/>
-      <c r="AG21" s="214"/>
-      <c r="AH21" s="215"/>
-    </row>
-    <row r="22" spans="5:34" ht="15" thickBot="1">
+    </row>
+    <row r="22" spans="5:25" ht="15" customHeight="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6615,27 +6602,20 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="216"/>
-      <c r="AC22" s="217"/>
-      <c r="AD22" s="217"/>
-      <c r="AE22" s="217"/>
-      <c r="AF22" s="217"/>
-      <c r="AG22" s="217"/>
-      <c r="AH22" s="218"/>
-    </row>
-    <row r="23" spans="5:34">
+    </row>
+    <row r="23" spans="5:25" ht="15">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="201" t="s">
+      <c r="F23" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="202" t="s">
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="202"/>
+      <c r="J23" s="214"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6658,7 +6638,7 @@
       <c r="X23" s="18"/>
       <c r="Y23" s="46"/>
     </row>
-    <row r="24" spans="5:34">
+    <row r="24" spans="5:25">
       <c r="E24" s="62" t="s">
         <v>23</v>
       </c>
@@ -6693,7 +6673,7 @@
       <c r="X24" s="18"/>
       <c r="Y24" s="46"/>
     </row>
-    <row r="25" spans="5:34">
+    <row r="25" spans="5:25">
       <c r="E25" s="63" t="s">
         <v>59</v>
       </c>
@@ -6727,7 +6707,7 @@
       <c r="X25" s="18"/>
       <c r="Y25" s="46"/>
     </row>
-    <row r="26" spans="5:34">
+    <row r="26" spans="5:25">
       <c r="N26" s="16" t="s">
         <v>26</v>
       </c>
@@ -6749,7 +6729,7 @@
       <c r="X26" s="18"/>
       <c r="Y26" s="46"/>
     </row>
-    <row r="27" spans="5:34">
+    <row r="27" spans="5:25">
       <c r="N27" s="10" t="s">
         <v>27</v>
       </c>
@@ -6771,7 +6751,7 @@
       <c r="X27" s="18"/>
       <c r="Y27" s="46"/>
     </row>
-    <row r="28" spans="5:34">
+    <row r="28" spans="5:25">
       <c r="N28" s="10" t="s">
         <v>68</v>
       </c>
@@ -6793,7 +6773,7 @@
       <c r="X28" s="18"/>
       <c r="Y28" s="46"/>
     </row>
-    <row r="29" spans="5:34">
+    <row r="29" spans="5:25">
       <c r="N29" s="9" t="s">
         <v>71</v>
       </c>
@@ -6815,7 +6795,7 @@
       <c r="X29" s="18"/>
       <c r="Y29" s="46"/>
     </row>
-    <row r="30" spans="5:34">
+    <row r="30" spans="5:25">
       <c r="N30" s="54" t="s">
         <v>74</v>
       </c>
@@ -6837,7 +6817,7 @@
       <c r="X30" s="18"/>
       <c r="Y30" s="46"/>
     </row>
-    <row r="31" spans="5:34">
+    <row r="31" spans="5:25">
       <c r="N31" s="11" t="s">
         <v>77</v>
       </c>
@@ -6859,7 +6839,7 @@
       <c r="X31" s="18"/>
       <c r="Y31" s="46"/>
     </row>
-    <row r="32" spans="5:34">
+    <row r="32" spans="5:25">
       <c r="N32" s="12" t="s">
         <v>80</v>
       </c>
@@ -6926,7 +6906,7 @@
       <c r="Y34" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="A1:AF1"/>
@@ -6934,7 +6914,6 @@
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="AB20:AH22"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F22:H22"/>
@@ -6955,8 +6934,8 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AB27" sqref="AB27"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -7010,7 +6989,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -7103,14 +7082,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="204"/>
-      <c r="AI2" s="205"/>
+      <c r="AG2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="216"/>
+      <c r="AI2" s="217"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7254,8 +7233,8 @@
       <c r="N4" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="72" t="s">
-        <v>20</v>
+      <c r="O4" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>17</v>
@@ -7311,11 +7290,11 @@
       </c>
       <c r="AH4" s="1">
         <f>COUNTIF(B4:AE4,"U")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AI4" s="1">
         <f t="shared" ref="AI4:AI11" si="0">AG4-AH4</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1">
@@ -8444,18 +8423,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:34" ht="15" thickBot="1"/>
-    <row r="20" spans="5:34">
+    <row r="19" spans="5:25" ht="15"/>
+    <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="206" t="s">
+      <c r="F20" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206" t="s">
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="206"/>
+      <c r="J20" s="218"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8477,29 +8456,20 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="210" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC20" s="211"/>
-      <c r="AD20" s="211"/>
-      <c r="AE20" s="211"/>
-      <c r="AF20" s="211"/>
-      <c r="AG20" s="211"/>
-      <c r="AH20" s="212"/>
-    </row>
-    <row r="21" spans="5:34">
+    </row>
+    <row r="21" spans="5:25" ht="14.45" customHeight="1">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8521,27 +8491,20 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="213"/>
-      <c r="AC21" s="214"/>
-      <c r="AD21" s="214"/>
-      <c r="AE21" s="214"/>
-      <c r="AF21" s="214"/>
-      <c r="AG21" s="214"/>
-      <c r="AH21" s="215"/>
-    </row>
-    <row r="22" spans="5:34" ht="15" thickBot="1">
+    </row>
+    <row r="22" spans="5:25" ht="15" customHeight="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8563,27 +8526,20 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="216"/>
-      <c r="AC22" s="217"/>
-      <c r="AD22" s="217"/>
-      <c r="AE22" s="217"/>
-      <c r="AF22" s="217"/>
-      <c r="AG22" s="217"/>
-      <c r="AH22" s="218"/>
-    </row>
-    <row r="23" spans="5:34">
+    </row>
+    <row r="23" spans="5:25" ht="15">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="201" t="s">
+      <c r="F23" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="202" t="s">
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="202"/>
+      <c r="J23" s="214"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8606,7 +8562,7 @@
       <c r="X23" s="18"/>
       <c r="Y23" s="46"/>
     </row>
-    <row r="24" spans="5:34">
+    <row r="24" spans="5:25">
       <c r="E24" s="62" t="s">
         <v>23</v>
       </c>
@@ -8641,7 +8597,7 @@
       <c r="X24" s="18"/>
       <c r="Y24" s="46"/>
     </row>
-    <row r="25" spans="5:34">
+    <row r="25" spans="5:25">
       <c r="E25" s="63" t="s">
         <v>59</v>
       </c>
@@ -8675,7 +8631,7 @@
       <c r="X25" s="18"/>
       <c r="Y25" s="46"/>
     </row>
-    <row r="26" spans="5:34">
+    <row r="26" spans="5:25">
       <c r="N26" s="16" t="s">
         <v>26</v>
       </c>
@@ -8697,7 +8653,7 @@
       <c r="X26" s="18"/>
       <c r="Y26" s="46"/>
     </row>
-    <row r="27" spans="5:34">
+    <row r="27" spans="5:25">
       <c r="N27" s="10" t="s">
         <v>27</v>
       </c>
@@ -8719,7 +8675,7 @@
       <c r="X27" s="18"/>
       <c r="Y27" s="46"/>
     </row>
-    <row r="28" spans="5:34">
+    <row r="28" spans="5:25">
       <c r="N28" s="10" t="s">
         <v>68</v>
       </c>
@@ -8741,7 +8697,7 @@
       <c r="X28" s="18"/>
       <c r="Y28" s="46"/>
     </row>
-    <row r="29" spans="5:34">
+    <row r="29" spans="5:25">
       <c r="N29" s="9" t="s">
         <v>71</v>
       </c>
@@ -8763,7 +8719,7 @@
       <c r="X29" s="18"/>
       <c r="Y29" s="46"/>
     </row>
-    <row r="30" spans="5:34">
+    <row r="30" spans="5:25">
       <c r="N30" s="54" t="s">
         <v>74</v>
       </c>
@@ -8785,7 +8741,7 @@
       <c r="X30" s="18"/>
       <c r="Y30" s="46"/>
     </row>
-    <row r="31" spans="5:34">
+    <row r="31" spans="5:25">
       <c r="N31" s="11" t="s">
         <v>77</v>
       </c>
@@ -8807,7 +8763,7 @@
       <c r="X31" s="18"/>
       <c r="Y31" s="46"/>
     </row>
-    <row r="32" spans="5:34">
+    <row r="32" spans="5:25">
       <c r="N32" s="12" t="s">
         <v>80</v>
       </c>
@@ -8853,7 +8809,7 @@
     </row>
     <row r="34" spans="14:25" ht="15" thickBot="1">
       <c r="N34" s="14" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="O34" s="50" t="s">
         <v>87</v>
@@ -8874,7 +8830,7 @@
       <c r="Y34" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="A1:AE1"/>
@@ -8882,7 +8838,6 @@
     <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="AB20:AH22"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F22:H22"/>
@@ -8902,8 +8857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DFC48C-09FC-43B2-ADD0-28180192959C}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -8959,7 +8914,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -9055,14 +9010,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="219"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9265,7 +9220,7 @@
       </c>
       <c r="AH4" s="1">
         <f>'NOV25'!AI4</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
@@ -9273,7 +9228,7 @@
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -10438,15 +10393,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="206" t="s">
+      <c r="F20" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206" t="s">
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="206"/>
+      <c r="J20" s="218"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10468,29 +10423,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="210" t="s">
+      <c r="AB20" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="211"/>
-      <c r="AD20" s="211"/>
-      <c r="AE20" s="211"/>
-      <c r="AF20" s="211"/>
-      <c r="AG20" s="211"/>
-      <c r="AH20" s="212"/>
+      <c r="AC20" s="205"/>
+      <c r="AD20" s="205"/>
+      <c r="AE20" s="205"/>
+      <c r="AF20" s="205"/>
+      <c r="AG20" s="205"/>
+      <c r="AH20" s="206"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10512,27 +10467,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="213"/>
-      <c r="AC21" s="214"/>
-      <c r="AD21" s="214"/>
-      <c r="AE21" s="214"/>
-      <c r="AF21" s="214"/>
-      <c r="AG21" s="214"/>
-      <c r="AH21" s="215"/>
+      <c r="AB21" s="207"/>
+      <c r="AC21" s="208"/>
+      <c r="AD21" s="208"/>
+      <c r="AE21" s="208"/>
+      <c r="AF21" s="208"/>
+      <c r="AG21" s="208"/>
+      <c r="AH21" s="209"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10554,27 +10509,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="216"/>
-      <c r="AC22" s="217"/>
-      <c r="AD22" s="217"/>
-      <c r="AE22" s="217"/>
-      <c r="AF22" s="217"/>
-      <c r="AG22" s="217"/>
-      <c r="AH22" s="218"/>
+      <c r="AB22" s="210"/>
+      <c r="AC22" s="211"/>
+      <c r="AD22" s="211"/>
+      <c r="AE22" s="211"/>
+      <c r="AF22" s="211"/>
+      <c r="AG22" s="211"/>
+      <c r="AH22" s="212"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="201" t="s">
+      <c r="F23" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="202" t="s">
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="202"/>
+      <c r="J23" s="214"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10893,7 +10848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD49DDB-D0B9-44C2-B6E9-FDC92C8C2F85}">
   <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4:AE4"/>
     </sheetView>
   </sheetViews>
@@ -10905,40 +10860,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="234" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="234"/>
-      <c r="K1" s="234"/>
-      <c r="L1" s="234"/>
-      <c r="M1" s="234"/>
-      <c r="N1" s="234"/>
-      <c r="O1" s="234"/>
-      <c r="P1" s="234"/>
-      <c r="Q1" s="234"/>
-      <c r="R1" s="234"/>
-      <c r="S1" s="234"/>
-      <c r="T1" s="234"/>
-      <c r="U1" s="234"/>
-      <c r="V1" s="234"/>
-      <c r="W1" s="234"/>
-      <c r="X1" s="234"/>
-      <c r="Y1" s="234"/>
-      <c r="Z1" s="234"/>
-      <c r="AA1" s="234"/>
-      <c r="AB1" s="234"/>
-      <c r="AC1" s="234"/>
-      <c r="AD1" s="234"/>
-      <c r="AE1" s="234"/>
-      <c r="AF1" s="234"/>
+      <c r="A1" s="243" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="243"/>
+      <c r="I1" s="243"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="243"/>
+      <c r="M1" s="243"/>
+      <c r="N1" s="243"/>
+      <c r="O1" s="243"/>
+      <c r="P1" s="243"/>
+      <c r="Q1" s="243"/>
+      <c r="R1" s="243"/>
+      <c r="S1" s="243"/>
+      <c r="T1" s="243"/>
+      <c r="U1" s="243"/>
+      <c r="V1" s="243"/>
+      <c r="W1" s="243"/>
+      <c r="X1" s="243"/>
+      <c r="Y1" s="243"/>
+      <c r="Z1" s="243"/>
+      <c r="AA1" s="243"/>
+      <c r="AB1" s="243"/>
+      <c r="AC1" s="243"/>
+      <c r="AD1" s="243"/>
+      <c r="AE1" s="243"/>
+      <c r="AF1" s="243"/>
       <c r="AG1" s="159"/>
       <c r="AH1" s="159"/>
       <c r="AI1" s="159"/>
@@ -10949,7 +10904,7 @@
       <c r="AN1" s="159"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="235">
+      <c r="A2" s="244">
         <v>46023</v>
       </c>
       <c r="B2" s="161">
@@ -11076,19 +11031,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="236" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="237"/>
-      <c r="AJ2" s="237"/>
-      <c r="AL2" s="236" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM2" s="237"/>
-      <c r="AN2" s="237"/>
+      <c r="AH2" s="245" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="246"/>
+      <c r="AJ2" s="246"/>
+      <c r="AL2" s="245" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM2" s="246"/>
+      <c r="AN2" s="246"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="235"/>
+      <c r="A3" s="244"/>
       <c r="B3" s="161" t="str">
         <f t="shared" ref="B3:AF3" si="1">UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -11220,7 +11175,7 @@
         <v>11</v>
       </c>
       <c r="AJ3" s="164" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AL3" s="163">
         <v>2026</v>
@@ -11229,7 +11184,7 @@
         <v>11</v>
       </c>
       <c r="AN3" s="164" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:40" ht="15" customHeight="1">
@@ -12454,14 +12409,14 @@
     </row>
     <row r="16" spans="1:40">
       <c r="E16" s="174"/>
-      <c r="F16" s="238" t="s">
+      <c r="F16" s="247" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="239"/>
-      <c r="H16" s="238" t="s">
+      <c r="G16" s="248"/>
+      <c r="H16" s="247" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="240"/>
+      <c r="I16" s="249"/>
       <c r="M16" s="168" t="s">
         <v>17</v>
       </c>
@@ -12487,14 +12442,14 @@
       <c r="E17" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="241" t="s">
+      <c r="F17" s="240" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="242"/>
-      <c r="H17" s="241" t="s">
+      <c r="G17" s="241"/>
+      <c r="H17" s="240" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="243"/>
+      <c r="I17" s="242"/>
       <c r="M17" s="181" t="s">
         <v>42</v>
       </c>
@@ -12520,14 +12475,14 @@
       <c r="E18" s="166" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="244" t="s">
+      <c r="F18" s="234" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="245"/>
-      <c r="H18" s="244" t="s">
+      <c r="G18" s="235"/>
+      <c r="H18" s="234" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="246"/>
+      <c r="I18" s="236"/>
       <c r="M18" s="161" t="s">
         <v>15</v>
       </c>
@@ -12553,14 +12508,14 @@
       <c r="E19" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="244" t="s">
+      <c r="F19" s="234" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="245"/>
-      <c r="H19" s="244" t="s">
+      <c r="G19" s="235"/>
+      <c r="H19" s="234" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="246"/>
+      <c r="I19" s="236"/>
       <c r="M19" s="187" t="s">
         <v>26</v>
       </c>
@@ -12581,28 +12536,28 @@
       <c r="V19" s="183"/>
       <c r="W19" s="183"/>
       <c r="X19" s="184"/>
-      <c r="AD19" s="210" t="s">
+      <c r="AD19" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AE19" s="211"/>
-      <c r="AF19" s="211"/>
-      <c r="AG19" s="211"/>
-      <c r="AH19" s="211"/>
-      <c r="AI19" s="211"/>
-      <c r="AJ19" s="212"/>
+      <c r="AE19" s="205"/>
+      <c r="AF19" s="205"/>
+      <c r="AG19" s="205"/>
+      <c r="AH19" s="205"/>
+      <c r="AI19" s="205"/>
+      <c r="AJ19" s="206"/>
     </row>
     <row r="20" spans="5:36">
       <c r="E20" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="244" t="s">
+      <c r="F20" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="245"/>
-      <c r="H20" s="244" t="s">
+      <c r="G20" s="235"/>
+      <c r="H20" s="234" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="246"/>
+      <c r="I20" s="236"/>
       <c r="M20" s="187" t="s">
         <v>18</v>
       </c>
@@ -12623,26 +12578,26 @@
       <c r="V20" s="183"/>
       <c r="W20" s="183"/>
       <c r="X20" s="184"/>
-      <c r="AD20" s="213"/>
-      <c r="AE20" s="214"/>
-      <c r="AF20" s="214"/>
-      <c r="AG20" s="214"/>
-      <c r="AH20" s="214"/>
-      <c r="AI20" s="214"/>
-      <c r="AJ20" s="215"/>
+      <c r="AD20" s="207"/>
+      <c r="AE20" s="208"/>
+      <c r="AF20" s="208"/>
+      <c r="AG20" s="208"/>
+      <c r="AH20" s="208"/>
+      <c r="AI20" s="208"/>
+      <c r="AJ20" s="209"/>
     </row>
     <row r="21" spans="5:36" ht="13.5" thickBot="1">
       <c r="E21" s="188" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="247" t="s">
+      <c r="F21" s="237" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="248"/>
-      <c r="H21" s="247" t="s">
+      <c r="G21" s="238"/>
+      <c r="H21" s="237" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="249"/>
+      <c r="I21" s="239"/>
       <c r="M21" s="189" t="s">
         <v>15</v>
       </c>
@@ -12663,13 +12618,13 @@
       <c r="V21" s="183"/>
       <c r="W21" s="183"/>
       <c r="X21" s="184"/>
-      <c r="AD21" s="216"/>
-      <c r="AE21" s="217"/>
-      <c r="AF21" s="217"/>
-      <c r="AG21" s="217"/>
-      <c r="AH21" s="217"/>
-      <c r="AI21" s="217"/>
-      <c r="AJ21" s="218"/>
+      <c r="AD21" s="210"/>
+      <c r="AE21" s="211"/>
+      <c r="AF21" s="211"/>
+      <c r="AG21" s="211"/>
+      <c r="AH21" s="211"/>
+      <c r="AI21" s="211"/>
+      <c r="AJ21" s="212"/>
     </row>
     <row r="22" spans="5:36">
       <c r="M22" s="189" t="s">
@@ -12871,23 +12826,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="AD19:AJ21"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="AD19:AJ21"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -12935,40 +12890,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
-      <c r="J1" s="221"/>
-      <c r="K1" s="221"/>
-      <c r="L1" s="221"/>
-      <c r="M1" s="221"/>
-      <c r="N1" s="221"/>
-      <c r="O1" s="221"/>
-      <c r="P1" s="221"/>
-      <c r="Q1" s="221"/>
-      <c r="R1" s="221"/>
-      <c r="S1" s="221"/>
-      <c r="T1" s="221"/>
-      <c r="U1" s="221"/>
-      <c r="V1" s="221"/>
-      <c r="W1" s="221"/>
-      <c r="X1" s="221"/>
-      <c r="Y1" s="221"/>
-      <c r="Z1" s="221"/>
-      <c r="AA1" s="220"/>
-      <c r="AB1" s="220"/>
-      <c r="AC1" s="220"/>
+      <c r="A1" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="220"/>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220"/>
+      <c r="J1" s="220"/>
+      <c r="K1" s="220"/>
+      <c r="L1" s="220"/>
+      <c r="M1" s="220"/>
+      <c r="N1" s="220"/>
+      <c r="O1" s="220"/>
+      <c r="P1" s="220"/>
+      <c r="Q1" s="220"/>
+      <c r="R1" s="220"/>
+      <c r="S1" s="220"/>
+      <c r="T1" s="220"/>
+      <c r="U1" s="220"/>
+      <c r="V1" s="220"/>
+      <c r="W1" s="220"/>
+      <c r="X1" s="220"/>
+      <c r="Y1" s="220"/>
+      <c r="Z1" s="220"/>
+      <c r="AA1" s="219"/>
+      <c r="AB1" s="219"/>
+      <c r="AC1" s="219"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -13055,19 +13010,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="204"/>
-      <c r="AG2" s="205"/>
-      <c r="AI2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="204"/>
-      <c r="AK2" s="205"/>
+      <c r="AE2" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="216"/>
+      <c r="AG2" s="217"/>
+      <c r="AI2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="216"/>
+      <c r="AK2" s="217"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="219"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -14317,15 +14272,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14347,29 +14302,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="210" t="s">
+      <c r="AB19" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="211"/>
-      <c r="AD19" s="211"/>
-      <c r="AE19" s="211"/>
-      <c r="AF19" s="211"/>
-      <c r="AG19" s="211"/>
-      <c r="AH19" s="212"/>
+      <c r="AC19" s="205"/>
+      <c r="AD19" s="205"/>
+      <c r="AE19" s="205"/>
+      <c r="AF19" s="205"/>
+      <c r="AG19" s="205"/>
+      <c r="AH19" s="206"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14391,27 +14346,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="213"/>
-      <c r="AC20" s="214"/>
-      <c r="AD20" s="214"/>
-      <c r="AE20" s="214"/>
-      <c r="AF20" s="214"/>
-      <c r="AG20" s="214"/>
-      <c r="AH20" s="215"/>
+      <c r="AB20" s="207"/>
+      <c r="AC20" s="208"/>
+      <c r="AD20" s="208"/>
+      <c r="AE20" s="208"/>
+      <c r="AF20" s="208"/>
+      <c r="AG20" s="208"/>
+      <c r="AH20" s="209"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14433,27 +14388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="216"/>
-      <c r="AC21" s="217"/>
-      <c r="AD21" s="217"/>
-      <c r="AE21" s="217"/>
-      <c r="AF21" s="217"/>
-      <c r="AG21" s="217"/>
-      <c r="AH21" s="218"/>
+      <c r="AB21" s="210"/>
+      <c r="AC21" s="211"/>
+      <c r="AD21" s="211"/>
+      <c r="AE21" s="211"/>
+      <c r="AF21" s="211"/>
+      <c r="AG21" s="211"/>
+      <c r="AH21" s="212"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14745,6 +14700,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -14753,11 +14713,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
@@ -14833,7 +14788,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -14929,19 +14884,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
-      <c r="AL2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="204"/>
-      <c r="AN2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
+      <c r="AL2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="216"/>
+      <c r="AN2" s="217"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -16303,15 +16258,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -16345,15 +16300,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16387,15 +16342,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16429,15 +16384,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16815,7 +16770,7 @@
       <c r="AE1" s="222"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -16908,19 +16863,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="204"/>
-      <c r="AI2" s="205"/>
-      <c r="AK2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="204"/>
-      <c r="AM2" s="205"/>
+      <c r="AG2" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="216"/>
+      <c r="AI2" s="217"/>
+      <c r="AK2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="216"/>
+      <c r="AM2" s="217"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -18241,15 +18196,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -18283,15 +18238,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -18325,15 +18280,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -18367,15 +18322,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18667,6 +18622,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -18674,11 +18634,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -18751,7 +18706,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -18847,14 +18802,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -20125,15 +20080,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -20155,29 +20110,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="210" t="s">
+      <c r="AB19" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="211"/>
-      <c r="AD19" s="211"/>
-      <c r="AE19" s="211"/>
-      <c r="AF19" s="211"/>
-      <c r="AG19" s="211"/>
-      <c r="AH19" s="212"/>
+      <c r="AC19" s="205"/>
+      <c r="AD19" s="205"/>
+      <c r="AE19" s="205"/>
+      <c r="AF19" s="205"/>
+      <c r="AG19" s="205"/>
+      <c r="AH19" s="206"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -20199,27 +20154,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="213"/>
-      <c r="AC20" s="214"/>
-      <c r="AD20" s="214"/>
-      <c r="AE20" s="214"/>
-      <c r="AF20" s="214"/>
-      <c r="AG20" s="214"/>
-      <c r="AH20" s="215"/>
+      <c r="AB20" s="207"/>
+      <c r="AC20" s="208"/>
+      <c r="AD20" s="208"/>
+      <c r="AE20" s="208"/>
+      <c r="AF20" s="208"/>
+      <c r="AG20" s="208"/>
+      <c r="AH20" s="209"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -20241,27 +20196,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="216"/>
-      <c r="AC21" s="217"/>
-      <c r="AD21" s="217"/>
-      <c r="AE21" s="217"/>
-      <c r="AF21" s="217"/>
-      <c r="AG21" s="217"/>
-      <c r="AH21" s="218"/>
+      <c r="AB21" s="210"/>
+      <c r="AC21" s="211"/>
+      <c r="AD21" s="211"/>
+      <c r="AE21" s="211"/>
+      <c r="AF21" s="211"/>
+      <c r="AG21" s="211"/>
+      <c r="AH21" s="212"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20553,18 +20508,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AB19:AH21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -20600,42 +20555,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221"/>
-      <c r="J1" s="221"/>
-      <c r="K1" s="221"/>
-      <c r="L1" s="221"/>
-      <c r="M1" s="221"/>
-      <c r="N1" s="221"/>
-      <c r="O1" s="221"/>
-      <c r="P1" s="221"/>
-      <c r="Q1" s="221"/>
-      <c r="R1" s="221"/>
-      <c r="S1" s="221"/>
-      <c r="T1" s="221"/>
-      <c r="U1" s="221"/>
-      <c r="V1" s="221"/>
-      <c r="W1" s="221"/>
-      <c r="X1" s="221"/>
-      <c r="Y1" s="221"/>
-      <c r="Z1" s="221"/>
-      <c r="AA1" s="221"/>
-      <c r="AB1" s="221"/>
-      <c r="AC1" s="221"/>
-      <c r="AD1" s="221"/>
-      <c r="AE1" s="221"/>
+      <c r="A1" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="220"/>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220"/>
+      <c r="J1" s="220"/>
+      <c r="K1" s="220"/>
+      <c r="L1" s="220"/>
+      <c r="M1" s="220"/>
+      <c r="N1" s="220"/>
+      <c r="O1" s="220"/>
+      <c r="P1" s="220"/>
+      <c r="Q1" s="220"/>
+      <c r="R1" s="220"/>
+      <c r="S1" s="220"/>
+      <c r="T1" s="220"/>
+      <c r="U1" s="220"/>
+      <c r="V1" s="220"/>
+      <c r="W1" s="220"/>
+      <c r="X1" s="220"/>
+      <c r="Y1" s="220"/>
+      <c r="Z1" s="220"/>
+      <c r="AA1" s="220"/>
+      <c r="AB1" s="220"/>
+      <c r="AC1" s="220"/>
+      <c r="AD1" s="220"/>
+      <c r="AE1" s="220"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -20728,14 +20683,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="204"/>
-      <c r="AI2" s="205"/>
+      <c r="AG2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="216"/>
+      <c r="AI2" s="217"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -21969,15 +21924,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -22004,15 +21959,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -22039,15 +21994,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -22074,15 +22029,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -22458,7 +22413,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -22554,14 +22509,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -23861,15 +23816,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="206" t="s">
+      <c r="F20" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206" t="s">
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="206"/>
+      <c r="J20" s="218"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -23896,15 +23851,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -23931,15 +23886,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -23966,15 +23921,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="201" t="s">
+      <c r="F23" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="202" t="s">
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="202"/>
+      <c r="J23" s="214"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -24349,7 +24304,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -24445,14 +24400,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="205"/>
+      <c r="AH2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="217"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="219"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -25722,15 +25677,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="206" t="s">
+      <c r="F19" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206" t="s">
+      <c r="G19" s="218"/>
+      <c r="H19" s="218"/>
+      <c r="I19" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="206"/>
+      <c r="J19" s="218"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -25752,29 +25707,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="210" t="s">
+      <c r="AB19" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="211"/>
-      <c r="AD19" s="211"/>
-      <c r="AE19" s="211"/>
-      <c r="AF19" s="211"/>
-      <c r="AG19" s="211"/>
-      <c r="AH19" s="212"/>
+      <c r="AC19" s="205"/>
+      <c r="AD19" s="205"/>
+      <c r="AE19" s="205"/>
+      <c r="AF19" s="205"/>
+      <c r="AG19" s="205"/>
+      <c r="AH19" s="206"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="201" t="s">
+      <c r="F20" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202" t="s">
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="202"/>
+      <c r="J20" s="214"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -25796,27 +25751,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="213"/>
-      <c r="AC20" s="214"/>
-      <c r="AD20" s="214"/>
-      <c r="AE20" s="214"/>
-      <c r="AF20" s="214"/>
-      <c r="AG20" s="214"/>
-      <c r="AH20" s="215"/>
+      <c r="AB20" s="207"/>
+      <c r="AC20" s="208"/>
+      <c r="AD20" s="208"/>
+      <c r="AE20" s="208"/>
+      <c r="AF20" s="208"/>
+      <c r="AG20" s="208"/>
+      <c r="AH20" s="209"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -25838,27 +25793,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="216"/>
-      <c r="AC21" s="217"/>
-      <c r="AD21" s="217"/>
-      <c r="AE21" s="217"/>
-      <c r="AF21" s="217"/>
-      <c r="AG21" s="217"/>
-      <c r="AH21" s="218"/>
+      <c r="AB21" s="210"/>
+      <c r="AC21" s="211"/>
+      <c r="AD21" s="211"/>
+      <c r="AE21" s="211"/>
+      <c r="AF21" s="211"/>
+      <c r="AG21" s="211"/>
+      <c r="AH21" s="212"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -26236,7 +26191,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="208">
+      <c r="A2" s="202">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -26329,14 +26284,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="203" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="204"/>
-      <c r="AI2" s="205"/>
+      <c r="AG2" s="215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="216"/>
+      <c r="AI2" s="217"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="209"/>
+      <c r="A3" s="203"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -27657,15 +27612,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="206" t="s">
+      <c r="F20" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206" t="s">
+      <c r="G20" s="218"/>
+      <c r="H20" s="218"/>
+      <c r="I20" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="206"/>
+      <c r="J20" s="218"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -27687,29 +27642,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="210" t="s">
+      <c r="AB20" s="204" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="211"/>
-      <c r="AD20" s="211"/>
-      <c r="AE20" s="211"/>
-      <c r="AF20" s="211"/>
-      <c r="AG20" s="211"/>
-      <c r="AH20" s="212"/>
+      <c r="AC20" s="205"/>
+      <c r="AD20" s="205"/>
+      <c r="AE20" s="205"/>
+      <c r="AF20" s="205"/>
+      <c r="AG20" s="205"/>
+      <c r="AH20" s="206"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="201" t="s">
+      <c r="F21" s="213" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="202"/>
-      <c r="H21" s="202"/>
-      <c r="I21" s="202" t="s">
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="202"/>
+      <c r="J21" s="214"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -27731,27 +27686,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="213"/>
-      <c r="AC21" s="214"/>
-      <c r="AD21" s="214"/>
-      <c r="AE21" s="214"/>
-      <c r="AF21" s="214"/>
-      <c r="AG21" s="214"/>
-      <c r="AH21" s="215"/>
+      <c r="AB21" s="207"/>
+      <c r="AC21" s="208"/>
+      <c r="AD21" s="208"/>
+      <c r="AE21" s="208"/>
+      <c r="AF21" s="208"/>
+      <c r="AG21" s="208"/>
+      <c r="AH21" s="209"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="201" t="s">
+      <c r="F22" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202" t="s">
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="202"/>
+      <c r="J22" s="214"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -27773,27 +27728,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="216"/>
-      <c r="AC22" s="217"/>
-      <c r="AD22" s="217"/>
-      <c r="AE22" s="217"/>
-      <c r="AF22" s="217"/>
-      <c r="AG22" s="217"/>
-      <c r="AH22" s="218"/>
+      <c r="AB22" s="210"/>
+      <c r="AC22" s="211"/>
+      <c r="AD22" s="211"/>
+      <c r="AE22" s="211"/>
+      <c r="AF22" s="211"/>
+      <c r="AG22" s="211"/>
+      <c r="AH22" s="212"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="201" t="s">
+      <c r="F23" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="202" t="s">
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="202"/>
+      <c r="J23" s="214"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -28123,6 +28078,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d1937d80d0a8e7ce848d3cb8198551">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1e82be046e0f9abcd1fd76bc3d6d064" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -28363,70 +28380,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28434,5 +28389,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-11-07 18:39:38 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="12" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2237,6 +2237,24 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2273,31 +2291,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2336,33 +2336,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2382,6 +2355,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3016,43 +3016,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
-      <c r="V1" s="201"/>
-      <c r="W1" s="201"/>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="201"/>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="201"/>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="201"/>
-      <c r="AD1" s="201"/>
-      <c r="AE1" s="201"/>
-      <c r="AF1" s="201"/>
+      <c r="A1" s="207" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="207"/>
+      <c r="I1" s="207"/>
+      <c r="J1" s="207"/>
+      <c r="K1" s="207"/>
+      <c r="L1" s="207"/>
+      <c r="M1" s="207"/>
+      <c r="N1" s="207"/>
+      <c r="O1" s="207"/>
+      <c r="P1" s="207"/>
+      <c r="Q1" s="207"/>
+      <c r="R1" s="207"/>
+      <c r="S1" s="207"/>
+      <c r="T1" s="207"/>
+      <c r="U1" s="207"/>
+      <c r="V1" s="207"/>
+      <c r="W1" s="207"/>
+      <c r="X1" s="207"/>
+      <c r="Y1" s="207"/>
+      <c r="Z1" s="207"/>
+      <c r="AA1" s="207"/>
+      <c r="AB1" s="207"/>
+      <c r="AC1" s="207"/>
+      <c r="AD1" s="207"/>
+      <c r="AE1" s="207"/>
+      <c r="AF1" s="207"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -3148,19 +3148,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
-      <c r="AL2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
+      <c r="AL2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="204"/>
+      <c r="AN2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4510,15 +4510,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4540,29 +4540,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4584,27 +4584,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4626,27 +4626,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4938,12 +4938,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4951,6 +4945,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
@@ -5023,7 +5023,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -5119,14 +5119,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6502,15 +6502,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6537,15 +6537,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6572,15 +6572,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6607,15 +6607,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6934,8 +6934,8 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AB27" sqref="AB27"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -6989,7 +6989,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -7082,14 +7082,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7646,14 +7646,14 @@
       <c r="I8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="83" t="s">
-        <v>26</v>
+      <c r="J8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="81" t="s">
+        <v>21</v>
       </c>
       <c r="M8" s="123" t="s">
         <v>17</v>
@@ -7661,17 +7661,17 @@
       <c r="N8" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="83" t="s">
-        <v>26</v>
+      <c r="O8" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="82" t="s">
+        <v>23</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>17</v>
@@ -7679,20 +7679,20 @@
       <c r="T8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="V8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="W8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="X8" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y8" s="83" t="s">
-        <v>26</v>
+      <c r="U8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="V8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="W8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="X8" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y8" s="81" t="s">
+        <v>21</v>
       </c>
       <c r="Z8" s="123" t="s">
         <v>17</v>
@@ -7718,11 +7718,11 @@
       </c>
       <c r="AH8" s="1">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:35" s="2" customFormat="1" ht="15" customHeight="1">
@@ -8211,15 +8211,15 @@
       </c>
       <c r="J14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="70">
         <f t="shared" si="5"/>
@@ -8255,23 +8255,23 @@
       </c>
       <c r="U14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y14" s="70">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z14" s="70">
         <f t="shared" si="5"/>
@@ -8356,19 +8356,19 @@
       </c>
       <c r="O15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S15" s="70">
         <f t="shared" si="6"/>
@@ -8426,15 +8426,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8461,15 +8461,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8496,15 +8496,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8531,15 +8531,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8857,8 +8857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DFC48C-09FC-43B2-ADD0-28180192959C}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="AJ18" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -8914,7 +8914,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -9010,14 +9010,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="AH8" s="1">
         <f>'NOV25'!AI8</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="AI8" s="1">
         <f>COUNTIF(B8:AF8,"U")</f>
@@ -9668,7 +9668,7 @@
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:36" s="2" customFormat="1" ht="15" customHeight="1">
@@ -10393,15 +10393,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10423,29 +10423,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10467,27 +10467,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10509,27 +10509,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10848,8 +10848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD49DDB-D0B9-44C2-B6E9-FDC92C8C2F85}">
   <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4:AE4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.95"/>
@@ -10860,40 +10860,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="243" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="243"/>
-      <c r="J1" s="243"/>
-      <c r="K1" s="243"/>
-      <c r="L1" s="243"/>
-      <c r="M1" s="243"/>
-      <c r="N1" s="243"/>
-      <c r="O1" s="243"/>
-      <c r="P1" s="243"/>
-      <c r="Q1" s="243"/>
-      <c r="R1" s="243"/>
-      <c r="S1" s="243"/>
-      <c r="T1" s="243"/>
-      <c r="U1" s="243"/>
-      <c r="V1" s="243"/>
-      <c r="W1" s="243"/>
-      <c r="X1" s="243"/>
-      <c r="Y1" s="243"/>
-      <c r="Z1" s="243"/>
-      <c r="AA1" s="243"/>
-      <c r="AB1" s="243"/>
-      <c r="AC1" s="243"/>
-      <c r="AD1" s="243"/>
-      <c r="AE1" s="243"/>
-      <c r="AF1" s="243"/>
+      <c r="A1" s="234" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="234"/>
+      <c r="C1" s="234"/>
+      <c r="D1" s="234"/>
+      <c r="E1" s="234"/>
+      <c r="F1" s="234"/>
+      <c r="G1" s="234"/>
+      <c r="H1" s="234"/>
+      <c r="I1" s="234"/>
+      <c r="J1" s="234"/>
+      <c r="K1" s="234"/>
+      <c r="L1" s="234"/>
+      <c r="M1" s="234"/>
+      <c r="N1" s="234"/>
+      <c r="O1" s="234"/>
+      <c r="P1" s="234"/>
+      <c r="Q1" s="234"/>
+      <c r="R1" s="234"/>
+      <c r="S1" s="234"/>
+      <c r="T1" s="234"/>
+      <c r="U1" s="234"/>
+      <c r="V1" s="234"/>
+      <c r="W1" s="234"/>
+      <c r="X1" s="234"/>
+      <c r="Y1" s="234"/>
+      <c r="Z1" s="234"/>
+      <c r="AA1" s="234"/>
+      <c r="AB1" s="234"/>
+      <c r="AC1" s="234"/>
+      <c r="AD1" s="234"/>
+      <c r="AE1" s="234"/>
+      <c r="AF1" s="234"/>
       <c r="AG1" s="159"/>
       <c r="AH1" s="159"/>
       <c r="AI1" s="159"/>
@@ -10904,7 +10904,7 @@
       <c r="AN1" s="159"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="244">
+      <c r="A2" s="235">
         <v>46023</v>
       </c>
       <c r="B2" s="161">
@@ -11031,19 +11031,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="245" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="246"/>
-      <c r="AJ2" s="246"/>
-      <c r="AL2" s="245" t="s">
+      <c r="AH2" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="237"/>
+      <c r="AJ2" s="237"/>
+      <c r="AL2" s="236" t="s">
         <v>104</v>
       </c>
-      <c r="AM2" s="246"/>
-      <c r="AN2" s="246"/>
+      <c r="AM2" s="237"/>
+      <c r="AN2" s="237"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="244"/>
+      <c r="A3" s="235"/>
       <c r="B3" s="161" t="str">
         <f t="shared" ref="B3:AF3" si="1">UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -11755,25 +11755,25 @@
       <c r="AC8" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="AD8" s="172" t="s">
-        <v>23</v>
+      <c r="AD8" s="187" t="s">
+        <v>18</v>
       </c>
       <c r="AE8" s="170" t="s">
         <v>27</v>
       </c>
-      <c r="AF8" s="172" t="s">
-        <v>23</v>
+      <c r="AF8" s="187" t="s">
+        <v>18</v>
       </c>
       <c r="AH8" s="168">
         <v>6</v>
       </c>
       <c r="AI8" s="169">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ8" s="169">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AL8" s="168">
         <v>22</v>
@@ -12396,7 +12396,7 @@
       </c>
       <c r="AD14" s="167">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="167">
         <f t="shared" si="7"/>
@@ -12404,19 +12404,19 @@
       </c>
       <c r="AF14" s="167">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:40">
       <c r="E16" s="174"/>
-      <c r="F16" s="247" t="s">
+      <c r="F16" s="238" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="248"/>
-      <c r="H16" s="247" t="s">
+      <c r="G16" s="239"/>
+      <c r="H16" s="238" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="249"/>
+      <c r="I16" s="240"/>
       <c r="M16" s="168" t="s">
         <v>17</v>
       </c>
@@ -12442,14 +12442,14 @@
       <c r="E17" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="240" t="s">
+      <c r="F17" s="241" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="241"/>
-      <c r="H17" s="240" t="s">
+      <c r="G17" s="242"/>
+      <c r="H17" s="241" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="242"/>
+      <c r="I17" s="243"/>
       <c r="M17" s="181" t="s">
         <v>42</v>
       </c>
@@ -12475,14 +12475,14 @@
       <c r="E18" s="166" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="234" t="s">
+      <c r="F18" s="244" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="235"/>
-      <c r="H18" s="234" t="s">
+      <c r="G18" s="245"/>
+      <c r="H18" s="244" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="236"/>
+      <c r="I18" s="246"/>
       <c r="M18" s="161" t="s">
         <v>15</v>
       </c>
@@ -12508,14 +12508,14 @@
       <c r="E19" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="234" t="s">
+      <c r="F19" s="244" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="235"/>
-      <c r="H19" s="234" t="s">
+      <c r="G19" s="245"/>
+      <c r="H19" s="244" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="236"/>
+      <c r="I19" s="246"/>
       <c r="M19" s="187" t="s">
         <v>26</v>
       </c>
@@ -12536,28 +12536,28 @@
       <c r="V19" s="183"/>
       <c r="W19" s="183"/>
       <c r="X19" s="184"/>
-      <c r="AD19" s="204" t="s">
+      <c r="AD19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="205"/>
-      <c r="AI19" s="205"/>
-      <c r="AJ19" s="206"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="211"/>
+      <c r="AI19" s="211"/>
+      <c r="AJ19" s="212"/>
     </row>
     <row r="20" spans="5:36">
       <c r="E20" s="172" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="234" t="s">
+      <c r="F20" s="244" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="235"/>
-      <c r="H20" s="234" t="s">
+      <c r="G20" s="245"/>
+      <c r="H20" s="244" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="236"/>
+      <c r="I20" s="246"/>
       <c r="M20" s="187" t="s">
         <v>18</v>
       </c>
@@ -12578,26 +12578,26 @@
       <c r="V20" s="183"/>
       <c r="W20" s="183"/>
       <c r="X20" s="184"/>
-      <c r="AD20" s="207"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="208"/>
-      <c r="AI20" s="208"/>
-      <c r="AJ20" s="209"/>
+      <c r="AD20" s="213"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="214"/>
+      <c r="AI20" s="214"/>
+      <c r="AJ20" s="215"/>
     </row>
     <row r="21" spans="5:36" ht="13.5" thickBot="1">
       <c r="E21" s="188" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="237" t="s">
+      <c r="F21" s="247" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="238"/>
-      <c r="H21" s="237" t="s">
+      <c r="G21" s="248"/>
+      <c r="H21" s="247" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="239"/>
+      <c r="I21" s="249"/>
       <c r="M21" s="189" t="s">
         <v>15</v>
       </c>
@@ -12618,13 +12618,13 @@
       <c r="V21" s="183"/>
       <c r="W21" s="183"/>
       <c r="X21" s="184"/>
-      <c r="AD21" s="210"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="211"/>
-      <c r="AI21" s="211"/>
-      <c r="AJ21" s="212"/>
+      <c r="AD21" s="216"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="217"/>
+      <c r="AI21" s="217"/>
+      <c r="AJ21" s="218"/>
     </row>
     <row r="22" spans="5:36">
       <c r="M22" s="189" t="s">
@@ -12826,23 +12826,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="AD19:AJ21"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AL2:AN2"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="AD19:AJ21"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -12890,40 +12890,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
-      <c r="T1" s="220"/>
-      <c r="U1" s="220"/>
-      <c r="V1" s="220"/>
-      <c r="W1" s="220"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="219"/>
-      <c r="AB1" s="219"/>
-      <c r="AC1" s="219"/>
+      <c r="A1" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="220"/>
+      <c r="AB1" s="220"/>
+      <c r="AC1" s="220"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -13010,19 +13010,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="216"/>
-      <c r="AG2" s="217"/>
-      <c r="AI2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="216"/>
-      <c r="AK2" s="217"/>
+      <c r="AE2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="204"/>
+      <c r="AG2" s="205"/>
+      <c r="AI2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="204"/>
+      <c r="AK2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -14272,15 +14272,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14302,29 +14302,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14346,27 +14346,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14388,27 +14388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14700,11 +14700,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -14713,6 +14708,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
@@ -14788,7 +14788,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -14884,19 +14884,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
-      <c r="AL2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
+      <c r="AL2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="204"/>
+      <c r="AN2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -16258,15 +16258,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -16300,15 +16300,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -16342,15 +16342,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16384,15 +16384,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16770,7 +16770,7 @@
       <c r="AE1" s="222"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -16863,19 +16863,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
-      <c r="AK2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="216"/>
-      <c r="AM2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
+      <c r="AK2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="204"/>
+      <c r="AM2" s="205"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -18196,15 +18196,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -18238,15 +18238,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -18280,15 +18280,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -18322,15 +18322,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18622,11 +18622,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -18634,6 +18629,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -18706,7 +18706,7 @@
       <c r="AF1" s="222"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -18802,14 +18802,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -20080,15 +20080,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -20110,29 +20110,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -20154,27 +20154,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -20196,27 +20196,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20508,18 +20508,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -20555,42 +20555,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
-      <c r="S1" s="220"/>
-      <c r="T1" s="220"/>
-      <c r="U1" s="220"/>
-      <c r="V1" s="220"/>
-      <c r="W1" s="220"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="220"/>
-      <c r="Z1" s="220"/>
-      <c r="AA1" s="220"/>
-      <c r="AB1" s="220"/>
-      <c r="AC1" s="220"/>
-      <c r="AD1" s="220"/>
-      <c r="AE1" s="220"/>
+      <c r="A1" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="221"/>
+      <c r="AB1" s="221"/>
+      <c r="AC1" s="221"/>
+      <c r="AD1" s="221"/>
+      <c r="AE1" s="221"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -20683,14 +20683,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -21924,15 +21924,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -21959,15 +21959,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -21994,15 +21994,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -22029,15 +22029,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -22413,7 +22413,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -22509,14 +22509,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -23816,15 +23816,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -23851,15 +23851,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -23886,15 +23886,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -23921,15 +23921,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -24304,7 +24304,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -24400,14 +24400,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="217"/>
+      <c r="AH2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="221"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -25677,15 +25677,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="218" t="s">
+      <c r="F19" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="218"/>
-      <c r="H19" s="218"/>
-      <c r="I19" s="218" t="s">
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="218"/>
+      <c r="J19" s="206"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -25707,29 +25707,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="204" t="s">
+      <c r="AB19" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="206"/>
+      <c r="AC19" s="211"/>
+      <c r="AD19" s="211"/>
+      <c r="AE19" s="211"/>
+      <c r="AF19" s="211"/>
+      <c r="AG19" s="211"/>
+      <c r="AH19" s="212"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="213" t="s">
+      <c r="F20" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214" t="s">
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="214"/>
+      <c r="J20" s="202"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -25751,27 +25751,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="207"/>
-      <c r="AC20" s="208"/>
-      <c r="AD20" s="208"/>
-      <c r="AE20" s="208"/>
-      <c r="AF20" s="208"/>
-      <c r="AG20" s="208"/>
-      <c r="AH20" s="209"/>
+      <c r="AB20" s="213"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="214"/>
+      <c r="AE20" s="214"/>
+      <c r="AF20" s="214"/>
+      <c r="AG20" s="214"/>
+      <c r="AH20" s="215"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -25793,27 +25793,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="210"/>
-      <c r="AC21" s="211"/>
-      <c r="AD21" s="211"/>
-      <c r="AE21" s="211"/>
-      <c r="AF21" s="211"/>
-      <c r="AG21" s="211"/>
-      <c r="AH21" s="212"/>
+      <c r="AB21" s="216"/>
+      <c r="AC21" s="217"/>
+      <c r="AD21" s="217"/>
+      <c r="AE21" s="217"/>
+      <c r="AF21" s="217"/>
+      <c r="AG21" s="217"/>
+      <c r="AH21" s="218"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -26191,7 +26191,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="202">
+      <c r="A2" s="208">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -26284,14 +26284,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="215" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="217"/>
+      <c r="AG2" s="203" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="204"/>
+      <c r="AI2" s="205"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="203"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -27612,15 +27612,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="218" t="s">
+      <c r="F20" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="218"/>
-      <c r="H20" s="218"/>
-      <c r="I20" s="218" t="s">
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="218"/>
+      <c r="J20" s="206"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -27642,29 +27642,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="204" t="s">
+      <c r="AB20" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="205"/>
-      <c r="AD20" s="205"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="205"/>
-      <c r="AG20" s="205"/>
-      <c r="AH20" s="206"/>
+      <c r="AC20" s="211"/>
+      <c r="AD20" s="211"/>
+      <c r="AE20" s="211"/>
+      <c r="AF20" s="211"/>
+      <c r="AG20" s="211"/>
+      <c r="AH20" s="212"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="213" t="s">
+      <c r="F21" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214" t="s">
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="214"/>
+      <c r="J21" s="202"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -27686,27 +27686,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="207"/>
-      <c r="AC21" s="208"/>
-      <c r="AD21" s="208"/>
-      <c r="AE21" s="208"/>
-      <c r="AF21" s="208"/>
-      <c r="AG21" s="208"/>
-      <c r="AH21" s="209"/>
+      <c r="AB21" s="213"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="214"/>
+      <c r="AE21" s="214"/>
+      <c r="AF21" s="214"/>
+      <c r="AG21" s="214"/>
+      <c r="AH21" s="215"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="213" t="s">
+      <c r="F22" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214" t="s">
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="214"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -27728,27 +27728,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="210"/>
-      <c r="AC22" s="211"/>
-      <c r="AD22" s="211"/>
-      <c r="AE22" s="211"/>
-      <c r="AF22" s="211"/>
-      <c r="AG22" s="211"/>
-      <c r="AH22" s="212"/>
+      <c r="AB22" s="216"/>
+      <c r="AC22" s="217"/>
+      <c r="AD22" s="217"/>
+      <c r="AE22" s="217"/>
+      <c r="AF22" s="217"/>
+      <c r="AG22" s="217"/>
+      <c r="AH22" s="218"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="213" t="s">
+      <c r="F23" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214" t="s">
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="214"/>
+      <c r="J23" s="202"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -28078,68 +28078,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d1937d80d0a8e7ce848d3cb8198551">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1e82be046e0f9abcd1fd76bc3d6d064" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -28380,8 +28318,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28389,5 +28389,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-02 18:48:42 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2036,6 +2036,27 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2072,31 +2093,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2133,9 +2136,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2736,43 +2736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="159" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
-      <c r="L1" s="159"/>
-      <c r="M1" s="159"/>
-      <c r="N1" s="159"/>
-      <c r="O1" s="159"/>
-      <c r="P1" s="159"/>
-      <c r="Q1" s="159"/>
-      <c r="R1" s="159"/>
-      <c r="S1" s="159"/>
-      <c r="T1" s="159"/>
-      <c r="U1" s="159"/>
-      <c r="V1" s="159"/>
-      <c r="W1" s="159"/>
-      <c r="X1" s="159"/>
-      <c r="Y1" s="159"/>
-      <c r="Z1" s="159"/>
-      <c r="AA1" s="159"/>
-      <c r="AB1" s="159"/>
-      <c r="AC1" s="159"/>
-      <c r="AD1" s="159"/>
-      <c r="AE1" s="159"/>
-      <c r="AF1" s="159"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+      <c r="AF1" s="166"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2868,19 +2868,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
-      <c r="AL2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="174"/>
-      <c r="AN2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4230,15 +4230,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4260,29 +4260,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="162" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="163"/>
-      <c r="AD19" s="163"/>
-      <c r="AE19" s="163"/>
-      <c r="AF19" s="163"/>
-      <c r="AG19" s="163"/>
-      <c r="AH19" s="164"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4304,27 +4304,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="165"/>
-      <c r="AC20" s="166"/>
-      <c r="AD20" s="166"/>
-      <c r="AE20" s="166"/>
-      <c r="AF20" s="166"/>
-      <c r="AG20" s="166"/>
-      <c r="AH20" s="167"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4346,27 +4346,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="168"/>
-      <c r="AC21" s="169"/>
-      <c r="AD21" s="169"/>
-      <c r="AE21" s="169"/>
-      <c r="AF21" s="169"/>
-      <c r="AG21" s="169"/>
-      <c r="AH21" s="170"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4658,12 +4658,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4671,6 +4665,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4703,47 +4703,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="184" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="184"/>
-      <c r="S1" s="184"/>
-      <c r="T1" s="184"/>
-      <c r="U1" s="184"/>
-      <c r="V1" s="184"/>
-      <c r="W1" s="184"/>
-      <c r="X1" s="184"/>
-      <c r="Y1" s="184"/>
-      <c r="Z1" s="184"/>
-      <c r="AA1" s="184"/>
-      <c r="AB1" s="184"/>
-      <c r="AC1" s="184"/>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="184"/>
+      <c r="A1" s="185" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="185"/>
+      <c r="P1" s="185"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="185"/>
+      <c r="V1" s="185"/>
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="185"/>
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="185"/>
+      <c r="AD1" s="185"/>
+      <c r="AE1" s="185"/>
+      <c r="AF1" s="185"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4839,14 +4839,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="179"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6222,15 +6222,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="176" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6257,15 +6257,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6292,15 +6292,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6327,15 +6327,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="171" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="172"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6653,9 +6653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1894A6B0-0132-46D2-8DB9-12FE5AD944BD}">
   <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AD20" sqref="AD20"/>
+      <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -6670,46 +6670,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
-      <c r="M1" s="186"/>
-      <c r="N1" s="186"/>
-      <c r="O1" s="186"/>
-      <c r="P1" s="186"/>
-      <c r="Q1" s="186"/>
-      <c r="R1" s="186"/>
-      <c r="S1" s="186"/>
-      <c r="T1" s="186"/>
-      <c r="U1" s="186"/>
-      <c r="V1" s="186"/>
-      <c r="W1" s="186"/>
-      <c r="X1" s="186"/>
-      <c r="Y1" s="186"/>
-      <c r="Z1" s="186"/>
-      <c r="AA1" s="186"/>
-      <c r="AB1" s="186"/>
-      <c r="AC1" s="186"/>
-      <c r="AD1" s="186"/>
-      <c r="AE1" s="186"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="187"/>
+      <c r="M1" s="187"/>
+      <c r="N1" s="187"/>
+      <c r="O1" s="187"/>
+      <c r="P1" s="187"/>
+      <c r="Q1" s="187"/>
+      <c r="R1" s="187"/>
+      <c r="S1" s="187"/>
+      <c r="T1" s="187"/>
+      <c r="U1" s="187"/>
+      <c r="V1" s="187"/>
+      <c r="W1" s="187"/>
+      <c r="X1" s="187"/>
+      <c r="Y1" s="187"/>
+      <c r="Z1" s="187"/>
+      <c r="AA1" s="187"/>
+      <c r="AB1" s="187"/>
+      <c r="AC1" s="187"/>
+      <c r="AD1" s="187"/>
+      <c r="AE1" s="187"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6802,14 +6802,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="174"/>
-      <c r="AI2" s="175"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -7608,31 +7608,31 @@
       <c r="R10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S10" s="192" t="s">
+      <c r="S10" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="T10" s="192" t="s">
+      <c r="T10" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="U10" s="192" t="s">
+      <c r="U10" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="123" t="s">
-        <v>17</v>
+      <c r="V10" s="159" t="s">
+        <v>16</v>
       </c>
       <c r="W10" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="X10" s="192" t="s">
+      <c r="X10" s="123" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="Y10" s="192" t="s">
+      <c r="Z10" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="Z10" s="192" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA10" s="192" t="s">
+      <c r="AA10" s="159" t="s">
         <v>16</v>
       </c>
       <c r="AB10" s="4" t="s">
@@ -8146,15 +8146,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="176" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8181,15 +8181,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8216,15 +8216,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8251,15 +8251,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="171" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="172"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8577,9 +8577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DFC48C-09FC-43B2-ADD0-28180192959C}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AJ18" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8594,47 +8594,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="189" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
-      <c r="H1" s="189"/>
-      <c r="I1" s="189"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="189"/>
-      <c r="M1" s="189"/>
-      <c r="N1" s="189"/>
-      <c r="O1" s="189"/>
-      <c r="P1" s="189"/>
-      <c r="Q1" s="190"/>
-      <c r="R1" s="190"/>
-      <c r="S1" s="189"/>
-      <c r="T1" s="189"/>
-      <c r="U1" s="189"/>
-      <c r="V1" s="189"/>
-      <c r="W1" s="189"/>
-      <c r="X1" s="190"/>
-      <c r="Y1" s="190"/>
-      <c r="Z1" s="189"/>
-      <c r="AA1" s="189"/>
-      <c r="AB1" s="189"/>
-      <c r="AC1" s="189"/>
-      <c r="AD1" s="189"/>
-      <c r="AE1" s="190"/>
-      <c r="AF1" s="191"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="190"/>
+      <c r="M1" s="190"/>
+      <c r="N1" s="190"/>
+      <c r="O1" s="190"/>
+      <c r="P1" s="190"/>
+      <c r="Q1" s="191"/>
+      <c r="R1" s="191"/>
+      <c r="S1" s="190"/>
+      <c r="T1" s="190"/>
+      <c r="U1" s="190"/>
+      <c r="V1" s="190"/>
+      <c r="W1" s="190"/>
+      <c r="X1" s="191"/>
+      <c r="Y1" s="191"/>
+      <c r="Z1" s="190"/>
+      <c r="AA1" s="190"/>
+      <c r="AB1" s="190"/>
+      <c r="AC1" s="190"/>
+      <c r="AD1" s="190"/>
+      <c r="AE1" s="191"/>
+      <c r="AF1" s="192"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8730,14 +8730,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="179"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -8848,17 +8848,17 @@
       <c r="B4" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="83" t="s">
-        <v>26</v>
+      <c r="C4" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
@@ -8944,11 +8944,11 @@
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -9069,7 +9069,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="72" t="s">
         <v>20</v>
@@ -10113,15 +10113,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="176" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10143,29 +10143,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="162" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="163"/>
-      <c r="AD20" s="163"/>
-      <c r="AE20" s="163"/>
-      <c r="AF20" s="163"/>
-      <c r="AG20" s="163"/>
-      <c r="AH20" s="164"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10187,27 +10187,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="165"/>
-      <c r="AC21" s="166"/>
-      <c r="AD21" s="166"/>
-      <c r="AE21" s="166"/>
-      <c r="AF21" s="166"/>
-      <c r="AG21" s="166"/>
-      <c r="AH21" s="167"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10229,27 +10229,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="168"/>
-      <c r="AC22" s="169"/>
-      <c r="AD22" s="169"/>
-      <c r="AE22" s="169"/>
-      <c r="AF22" s="169"/>
-      <c r="AG22" s="169"/>
-      <c r="AH22" s="170"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="171" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="172"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10592,40 +10592,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="177" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10712,19 +10712,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="174"/>
-      <c r="AG2" s="175"/>
-      <c r="AI2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="174"/>
-      <c r="AK2" s="175"/>
+      <c r="AE2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="163"/>
+      <c r="AG2" s="164"/>
+      <c r="AI2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="163"/>
+      <c r="AK2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="179"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -11974,15 +11974,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12004,29 +12004,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="162" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="163"/>
-      <c r="AD19" s="163"/>
-      <c r="AE19" s="163"/>
-      <c r="AF19" s="163"/>
-      <c r="AG19" s="163"/>
-      <c r="AH19" s="164"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12048,27 +12048,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="165"/>
-      <c r="AC20" s="166"/>
-      <c r="AD20" s="166"/>
-      <c r="AE20" s="166"/>
-      <c r="AF20" s="166"/>
-      <c r="AG20" s="166"/>
-      <c r="AH20" s="167"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12090,27 +12090,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="168"/>
-      <c r="AC21" s="169"/>
-      <c r="AD21" s="169"/>
-      <c r="AE21" s="169"/>
-      <c r="AF21" s="169"/>
-      <c r="AG21" s="169"/>
-      <c r="AH21" s="170"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12402,11 +12402,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12415,6 +12410,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12454,43 +12454,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="180" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
-      <c r="AF1" s="180"/>
+      <c r="A1" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12586,19 +12586,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
-      <c r="AL2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="174"/>
-      <c r="AN2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -13960,15 +13960,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14002,15 +14002,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14044,15 +14044,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14086,15 +14086,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14437,42 +14437,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="180" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
+      <c r="A1" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14565,19 +14565,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="173" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="174"/>
-      <c r="AI2" s="175"/>
-      <c r="AK2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="174"/>
-      <c r="AM2" s="175"/>
+      <c r="AG2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
+      <c r="AK2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="163"/>
+      <c r="AM2" s="164"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15898,15 +15898,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15940,15 +15940,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -15982,15 +15982,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16024,15 +16024,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16324,11 +16324,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16336,6 +16331,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16372,43 +16372,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="180" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
-      <c r="AF1" s="180"/>
+      <c r="A1" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16504,14 +16504,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17782,15 +17782,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17812,29 +17812,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="162" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="163"/>
-      <c r="AD19" s="163"/>
-      <c r="AE19" s="163"/>
-      <c r="AF19" s="163"/>
-      <c r="AG19" s="163"/>
-      <c r="AH19" s="164"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17856,27 +17856,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="165"/>
-      <c r="AC20" s="166"/>
-      <c r="AD20" s="166"/>
-      <c r="AE20" s="166"/>
-      <c r="AF20" s="166"/>
-      <c r="AG20" s="166"/>
-      <c r="AH20" s="167"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17898,27 +17898,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="168"/>
-      <c r="AC21" s="169"/>
-      <c r="AD21" s="169"/>
-      <c r="AE21" s="169"/>
-      <c r="AF21" s="169"/>
-      <c r="AG21" s="169"/>
-      <c r="AH21" s="170"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18210,18 +18210,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18257,42 +18257,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="177" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="180"/>
+      <c r="AB1" s="180"/>
+      <c r="AC1" s="180"/>
+      <c r="AD1" s="180"/>
+      <c r="AE1" s="180"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18385,14 +18385,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="174"/>
-      <c r="AI2" s="175"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19626,15 +19626,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19661,15 +19661,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19696,15 +19696,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19731,15 +19731,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20115,7 +20115,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20211,14 +20211,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -20582,25 +20582,25 @@
       <c r="M6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="181"/>
-      <c r="O6" s="182"/>
-      <c r="P6" s="182"/>
-      <c r="Q6" s="182"/>
-      <c r="R6" s="182"/>
-      <c r="S6" s="182"/>
-      <c r="T6" s="182"/>
-      <c r="U6" s="182"/>
-      <c r="V6" s="182"/>
-      <c r="W6" s="182"/>
-      <c r="X6" s="182"/>
-      <c r="Y6" s="182"/>
-      <c r="Z6" s="182"/>
-      <c r="AA6" s="182"/>
-      <c r="AB6" s="182"/>
-      <c r="AC6" s="182"/>
-      <c r="AD6" s="182"/>
-      <c r="AE6" s="182"/>
-      <c r="AF6" s="183"/>
+      <c r="N6" s="182"/>
+      <c r="O6" s="183"/>
+      <c r="P6" s="183"/>
+      <c r="Q6" s="183"/>
+      <c r="R6" s="183"/>
+      <c r="S6" s="183"/>
+      <c r="T6" s="183"/>
+      <c r="U6" s="183"/>
+      <c r="V6" s="183"/>
+      <c r="W6" s="183"/>
+      <c r="X6" s="183"/>
+      <c r="Y6" s="183"/>
+      <c r="Z6" s="183"/>
+      <c r="AA6" s="183"/>
+      <c r="AB6" s="183"/>
+      <c r="AC6" s="183"/>
+      <c r="AD6" s="183"/>
+      <c r="AE6" s="183"/>
+      <c r="AF6" s="184"/>
       <c r="AG6"/>
       <c r="AH6" s="1">
         <f>'JUN25'!AI6</f>
@@ -21518,15 +21518,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="176" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21553,15 +21553,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21588,15 +21588,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21623,15 +21623,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="171" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="172"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -21966,47 +21966,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="184" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
-      <c r="M1" s="185"/>
-      <c r="N1" s="185"/>
-      <c r="O1" s="185"/>
-      <c r="P1" s="185"/>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="185"/>
-      <c r="S1" s="185"/>
-      <c r="T1" s="185"/>
-      <c r="U1" s="185"/>
-      <c r="V1" s="185"/>
-      <c r="W1" s="185"/>
-      <c r="X1" s="185"/>
-      <c r="Y1" s="185"/>
-      <c r="Z1" s="185"/>
-      <c r="AA1" s="185"/>
-      <c r="AB1" s="185"/>
-      <c r="AC1" s="185"/>
-      <c r="AD1" s="185"/>
-      <c r="AE1" s="185"/>
-      <c r="AF1" s="185"/>
+      <c r="A1" s="185" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+      <c r="N1" s="186"/>
+      <c r="O1" s="186"/>
+      <c r="P1" s="186"/>
+      <c r="Q1" s="186"/>
+      <c r="R1" s="186"/>
+      <c r="S1" s="186"/>
+      <c r="T1" s="186"/>
+      <c r="U1" s="186"/>
+      <c r="V1" s="186"/>
+      <c r="W1" s="186"/>
+      <c r="X1" s="186"/>
+      <c r="Y1" s="186"/>
+      <c r="Z1" s="186"/>
+      <c r="AA1" s="186"/>
+      <c r="AB1" s="186"/>
+      <c r="AC1" s="186"/>
+      <c r="AD1" s="186"/>
+      <c r="AE1" s="186"/>
+      <c r="AF1" s="186"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22102,14 +22102,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="174"/>
-      <c r="AJ2" s="175"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="179"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23379,15 +23379,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="176" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="176"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23409,29 +23409,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="162" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="163"/>
-      <c r="AD19" s="163"/>
-      <c r="AE19" s="163"/>
-      <c r="AF19" s="163"/>
-      <c r="AG19" s="163"/>
-      <c r="AH19" s="164"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="171" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="172"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23453,27 +23453,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="165"/>
-      <c r="AC20" s="166"/>
-      <c r="AD20" s="166"/>
-      <c r="AE20" s="166"/>
-      <c r="AF20" s="166"/>
-      <c r="AG20" s="166"/>
-      <c r="AH20" s="167"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23495,27 +23495,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="168"/>
-      <c r="AC21" s="169"/>
-      <c r="AD21" s="169"/>
-      <c r="AE21" s="169"/>
-      <c r="AF21" s="169"/>
-      <c r="AG21" s="169"/>
-      <c r="AH21" s="170"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23854,46 +23854,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="186" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="187"/>
-      <c r="K1" s="187"/>
-      <c r="L1" s="187"/>
-      <c r="M1" s="187"/>
-      <c r="N1" s="187"/>
-      <c r="O1" s="187"/>
-      <c r="P1" s="187"/>
-      <c r="Q1" s="187"/>
-      <c r="R1" s="187"/>
-      <c r="S1" s="187"/>
-      <c r="T1" s="187"/>
-      <c r="U1" s="187"/>
-      <c r="V1" s="187"/>
-      <c r="W1" s="187"/>
-      <c r="X1" s="187"/>
-      <c r="Y1" s="187"/>
-      <c r="Z1" s="187"/>
-      <c r="AA1" s="187"/>
-      <c r="AB1" s="187"/>
-      <c r="AC1" s="187"/>
-      <c r="AD1" s="187"/>
-      <c r="AE1" s="187"/>
+      <c r="A1" s="187" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="188"/>
+      <c r="P1" s="188"/>
+      <c r="Q1" s="188"/>
+      <c r="R1" s="188"/>
+      <c r="S1" s="188"/>
+      <c r="T1" s="188"/>
+      <c r="U1" s="188"/>
+      <c r="V1" s="188"/>
+      <c r="W1" s="188"/>
+      <c r="X1" s="188"/>
+      <c r="Y1" s="188"/>
+      <c r="Z1" s="188"/>
+      <c r="AA1" s="188"/>
+      <c r="AB1" s="188"/>
+      <c r="AC1" s="188"/>
+      <c r="AD1" s="188"/>
+      <c r="AE1" s="188"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="160">
+      <c r="A2" s="167">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -23986,14 +23986,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="173" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="174"/>
-      <c r="AI2" s="175"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="161"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25314,15 +25314,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="176" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25344,29 +25344,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="162" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="163"/>
-      <c r="AD20" s="163"/>
-      <c r="AE20" s="163"/>
-      <c r="AF20" s="163"/>
-      <c r="AG20" s="163"/>
-      <c r="AH20" s="164"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="171" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="172"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25388,27 +25388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="165"/>
-      <c r="AC21" s="166"/>
-      <c r="AD21" s="166"/>
-      <c r="AE21" s="166"/>
-      <c r="AF21" s="166"/>
-      <c r="AG21" s="166"/>
-      <c r="AH21" s="167"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="171" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="172"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25430,27 +25430,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="168"/>
-      <c r="AC22" s="169"/>
-      <c r="AD22" s="169"/>
-      <c r="AE22" s="169"/>
-      <c r="AF22" s="169"/>
-      <c r="AG22" s="169"/>
-      <c r="AH22" s="170"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="171" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="172"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25780,8 +25780,70 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d1937d80d0a8e7ce848d3cb8198551">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e1e82be046e0f9abcd1fd76bc3d6d064" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64cef5f809c20957e1bed8db4fd8bd69">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9eb64a58f9f8c69f3f340dcbb635673" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
     <xsd:import namespace="fa453329-a4c9-4120-b786-6a0f9fa17d90"/>
     <xsd:element name="properties">
@@ -26020,70 +26082,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CB7833C-F101-415F-82FC-BD60669F23FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26091,5 +26091,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-04 18:48:12 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2039,24 +2039,6 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2093,13 +2075,31 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2736,43 +2736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="166" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="166"/>
-      <c r="AC1" s="166"/>
-      <c r="AD1" s="166"/>
-      <c r="AE1" s="166"/>
-      <c r="AF1" s="166"/>
+      <c r="A1" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+      <c r="Q1" s="160"/>
+      <c r="R1" s="160"/>
+      <c r="S1" s="160"/>
+      <c r="T1" s="160"/>
+      <c r="U1" s="160"/>
+      <c r="V1" s="160"/>
+      <c r="W1" s="160"/>
+      <c r="X1" s="160"/>
+      <c r="Y1" s="160"/>
+      <c r="Z1" s="160"/>
+      <c r="AA1" s="160"/>
+      <c r="AB1" s="160"/>
+      <c r="AC1" s="160"/>
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="160"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2868,19 +2868,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
-      <c r="AL2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="163"/>
-      <c r="AN2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
+      <c r="AL2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4230,15 +4230,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4260,29 +4260,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4304,27 +4304,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4346,27 +4346,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4658,6 +4658,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4665,12 +4671,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4743,7 +4743,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4839,14 +4839,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6222,15 +6222,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6257,15 +6257,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6292,15 +6292,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6327,15 +6327,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6709,7 +6709,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6802,14 +6802,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -8146,15 +8146,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8181,15 +8181,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8216,15 +8216,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8251,15 +8251,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8579,7 +8579,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8634,7 +8634,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8730,14 +8730,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9404,11 +9404,11 @@
       <c r="D9" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="82" t="s">
-        <v>23</v>
+      <c r="E9" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="G9" s="82" t="s">
         <v>23</v>
@@ -9495,11 +9495,11 @@
       </c>
       <c r="AI9" s="1">
         <f t="shared" ref="AI9:AI11" si="1">COUNTIF(B9:AF9,"U")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="15" customHeight="1">
@@ -9999,11 +9999,11 @@
       </c>
       <c r="E15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="70">
         <f t="shared" si="6"/>
@@ -10113,15 +10113,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10143,29 +10143,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="169" t="s">
+      <c r="AB20" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10187,27 +10187,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10229,27 +10229,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="175"/>
-      <c r="AC22" s="176"/>
-      <c r="AD22" s="176"/>
-      <c r="AE22" s="176"/>
-      <c r="AF22" s="176"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="177"/>
+      <c r="AB22" s="169"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="170"/>
+      <c r="AE22" s="170"/>
+      <c r="AF22" s="170"/>
+      <c r="AG22" s="170"/>
+      <c r="AH22" s="171"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10592,40 +10592,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="179" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
-      <c r="AC1" s="179"/>
+      <c r="A1" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10712,19 +10712,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="163"/>
-      <c r="AG2" s="164"/>
-      <c r="AI2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="163"/>
-      <c r="AK2" s="164"/>
+      <c r="AE2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="175"/>
+      <c r="AG2" s="176"/>
+      <c r="AI2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="175"/>
+      <c r="AK2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -11974,15 +11974,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12004,29 +12004,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12048,27 +12048,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12090,27 +12090,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12402,6 +12402,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12410,11 +12415,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12490,7 +12490,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12586,19 +12586,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
-      <c r="AL2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="163"/>
-      <c r="AN2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
+      <c r="AL2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -13960,15 +13960,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14002,15 +14002,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14044,15 +14044,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14086,15 +14086,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14472,7 +14472,7 @@
       <c r="AE1" s="181"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14565,19 +14565,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
-      <c r="AK2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="163"/>
-      <c r="AM2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
+      <c r="AK2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="175"/>
+      <c r="AM2" s="176"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15898,15 +15898,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15940,15 +15940,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -15982,15 +15982,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16024,15 +16024,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16324,6 +16324,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16331,11 +16336,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16408,7 +16408,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16504,14 +16504,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17782,15 +17782,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17812,29 +17812,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17856,27 +17856,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17898,27 +17898,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18210,18 +18210,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AB19:AH21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18257,42 +18257,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="179" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
+      <c r="A1" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18385,14 +18385,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19626,15 +19626,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19661,15 +19661,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19696,15 +19696,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19731,15 +19731,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20115,7 +20115,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20211,14 +20211,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21518,15 +21518,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21553,15 +21553,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21588,15 +21588,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21623,15 +21623,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22006,7 +22006,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22102,14 +22102,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23379,15 +23379,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23409,29 +23409,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23453,27 +23453,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23495,27 +23495,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23893,7 +23893,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -23986,14 +23986,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25314,15 +25314,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25344,29 +25344,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="169" t="s">
+      <c r="AB20" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25388,27 +25388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25430,27 +25430,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="175"/>
-      <c r="AC22" s="176"/>
-      <c r="AD22" s="176"/>
-      <c r="AE22" s="176"/>
-      <c r="AF22" s="176"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="177"/>
+      <c r="AB22" s="169"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="170"/>
+      <c r="AE22" s="170"/>
+      <c r="AF22" s="170"/>
+      <c r="AG22" s="170"/>
+      <c r="AH22" s="171"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25780,68 +25780,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64cef5f809c20957e1bed8db4fd8bd69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9eb64a58f9f8c69f3f340dcbb635673" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26082,8 +26020,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26091,5 +26091,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-05 18:41:39 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -2039,6 +2039,24 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2075,31 +2093,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2736,43 +2736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="160"/>
-      <c r="L1" s="160"/>
-      <c r="M1" s="160"/>
-      <c r="N1" s="160"/>
-      <c r="O1" s="160"/>
-      <c r="P1" s="160"/>
-      <c r="Q1" s="160"/>
-      <c r="R1" s="160"/>
-      <c r="S1" s="160"/>
-      <c r="T1" s="160"/>
-      <c r="U1" s="160"/>
-      <c r="V1" s="160"/>
-      <c r="W1" s="160"/>
-      <c r="X1" s="160"/>
-      <c r="Y1" s="160"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="160"/>
-      <c r="AB1" s="160"/>
-      <c r="AC1" s="160"/>
-      <c r="AD1" s="160"/>
-      <c r="AE1" s="160"/>
-      <c r="AF1" s="160"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+      <c r="AF1" s="166"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2868,19 +2868,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
-      <c r="AL2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="175"/>
-      <c r="AN2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4230,15 +4230,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4260,29 +4260,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4304,27 +4304,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4346,27 +4346,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4658,12 +4658,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4671,6 +4665,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4743,7 +4743,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4839,14 +4839,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6222,15 +6222,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6257,15 +6257,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6292,15 +6292,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6327,15 +6327,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6709,7 +6709,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6802,14 +6802,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -8146,15 +8146,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8181,15 +8181,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8216,15 +8216,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8251,15 +8251,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8579,7 +8579,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8634,7 +8634,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8730,14 +8730,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -9078,7 +9078,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="72" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>17</v>
@@ -10113,15 +10113,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10143,29 +10143,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="163" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10187,27 +10187,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10229,27 +10229,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="169"/>
-      <c r="AC22" s="170"/>
-      <c r="AD22" s="170"/>
-      <c r="AE22" s="170"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="170"/>
-      <c r="AH22" s="171"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10592,40 +10592,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="179"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="179"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10712,19 +10712,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="175"/>
-      <c r="AG2" s="176"/>
-      <c r="AI2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="175"/>
-      <c r="AK2" s="176"/>
+      <c r="AE2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="163"/>
+      <c r="AG2" s="164"/>
+      <c r="AI2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="163"/>
+      <c r="AK2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -11974,15 +11974,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12004,29 +12004,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12048,27 +12048,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12090,27 +12090,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12402,11 +12402,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12415,6 +12410,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12490,7 +12490,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12586,19 +12586,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
-      <c r="AL2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="175"/>
-      <c r="AN2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -13960,15 +13960,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14002,15 +14002,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14044,15 +14044,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14086,15 +14086,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14472,7 +14472,7 @@
       <c r="AE1" s="181"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14565,19 +14565,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
-      <c r="AK2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="175"/>
-      <c r="AM2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
+      <c r="AK2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="163"/>
+      <c r="AM2" s="164"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15898,15 +15898,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15940,15 +15940,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -15982,15 +15982,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16024,15 +16024,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16324,11 +16324,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16336,6 +16331,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16408,7 +16408,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16504,14 +16504,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17782,15 +17782,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17812,29 +17812,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17856,27 +17856,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17898,27 +17898,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18210,18 +18210,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18257,42 +18257,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="179"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="179"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
-      <c r="AC1" s="179"/>
-      <c r="AD1" s="179"/>
-      <c r="AE1" s="179"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="180"/>
+      <c r="AB1" s="180"/>
+      <c r="AC1" s="180"/>
+      <c r="AD1" s="180"/>
+      <c r="AE1" s="180"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18385,14 +18385,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19626,15 +19626,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19661,15 +19661,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19696,15 +19696,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19731,15 +19731,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20115,7 +20115,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20211,14 +20211,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21518,15 +21518,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21553,15 +21553,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21588,15 +21588,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21623,15 +21623,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22006,7 +22006,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22102,14 +22102,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23379,15 +23379,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23409,29 +23409,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23453,27 +23453,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23495,27 +23495,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23893,7 +23893,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -23986,14 +23986,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25314,15 +25314,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25344,29 +25344,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="163" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25388,27 +25388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25430,27 +25430,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="169"/>
-      <c r="AC22" s="170"/>
-      <c r="AD22" s="170"/>
-      <c r="AE22" s="170"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="170"/>
-      <c r="AH22" s="171"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25780,6 +25780,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64cef5f809c20957e1bed8db4fd8bd69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9eb64a58f9f8c69f3f340dcbb635673" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26020,70 +26082,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26091,5 +26091,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-08 18:46:29 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8578,8 +8578,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8866,8 +8866,8 @@
       <c r="H4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="98" t="s">
-        <v>15</v>
+      <c r="I4" s="72" t="s">
+        <v>20</v>
       </c>
       <c r="J4" s="72" t="s">
         <v>20</v>
@@ -9339,14 +9339,14 @@
       <c r="S8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="81" t="s">
-        <v>21</v>
+      <c r="T8" s="123" t="s">
+        <v>17</v>
       </c>
       <c r="U8" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="123" t="s">
-        <v>17</v>
+      <c r="V8" s="82" t="s">
+        <v>23</v>
       </c>
       <c r="W8" s="82" t="s">
         <v>23</v>
@@ -9557,20 +9557,20 @@
       <c r="R10" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="S10" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="T10" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="U10" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="V10" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="W10" s="82" t="s">
-        <v>23</v>
+      <c r="S10" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>17</v>
@@ -9605,11 +9605,11 @@
       </c>
       <c r="AI10" s="1">
         <f t="shared" ref="AI10" si="2">COUNTIF(B10:AF10,"U")</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AJ10" s="1">
         <f t="shared" ref="AJ10" si="3">AH10-AI10</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="15" customHeight="1">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="T14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U14" s="70">
         <f t="shared" si="5"/>
@@ -10055,15 +10055,15 @@
       </c>
       <c r="S15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V15" s="70">
         <f t="shared" si="6"/>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="W15" s="70">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X15" s="70">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Update files and calendar (2025-12-09 18:41:59 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -2039,24 +2039,6 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2093,13 +2075,31 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2736,43 +2736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="166" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="166"/>
-      <c r="AC1" s="166"/>
-      <c r="AD1" s="166"/>
-      <c r="AE1" s="166"/>
-      <c r="AF1" s="166"/>
+      <c r="A1" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+      <c r="Q1" s="160"/>
+      <c r="R1" s="160"/>
+      <c r="S1" s="160"/>
+      <c r="T1" s="160"/>
+      <c r="U1" s="160"/>
+      <c r="V1" s="160"/>
+      <c r="W1" s="160"/>
+      <c r="X1" s="160"/>
+      <c r="Y1" s="160"/>
+      <c r="Z1" s="160"/>
+      <c r="AA1" s="160"/>
+      <c r="AB1" s="160"/>
+      <c r="AC1" s="160"/>
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="160"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2868,19 +2868,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
-      <c r="AL2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="163"/>
-      <c r="AN2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
+      <c r="AL2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4230,15 +4230,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4260,29 +4260,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4304,27 +4304,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4346,27 +4346,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4658,6 +4658,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4665,12 +4671,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4743,7 +4743,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4839,14 +4839,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6222,15 +6222,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6257,15 +6257,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6292,15 +6292,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6327,15 +6327,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6709,7 +6709,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6802,14 +6802,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -8146,15 +8146,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8181,15 +8181,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8216,15 +8216,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8251,15 +8251,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8578,8 +8578,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="N21" sqref="N21"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8634,7 +8634,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8730,14 +8730,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -8875,8 +8875,8 @@
       <c r="K4" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="72" t="s">
-        <v>20</v>
+      <c r="L4" s="81" t="s">
+        <v>21</v>
       </c>
       <c r="M4" s="72" t="s">
         <v>20</v>
@@ -9898,7 +9898,7 @@
       </c>
       <c r="L14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" s="70">
         <f t="shared" si="5"/>
@@ -10113,15 +10113,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10143,29 +10143,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="169" t="s">
+      <c r="AB20" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10187,27 +10187,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10229,27 +10229,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="175"/>
-      <c r="AC22" s="176"/>
-      <c r="AD22" s="176"/>
-      <c r="AE22" s="176"/>
-      <c r="AF22" s="176"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="177"/>
+      <c r="AB22" s="169"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="170"/>
+      <c r="AE22" s="170"/>
+      <c r="AF22" s="170"/>
+      <c r="AG22" s="170"/>
+      <c r="AH22" s="171"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10592,40 +10592,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="179" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
-      <c r="AC1" s="179"/>
+      <c r="A1" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10712,19 +10712,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="163"/>
-      <c r="AG2" s="164"/>
-      <c r="AI2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="163"/>
-      <c r="AK2" s="164"/>
+      <c r="AE2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="175"/>
+      <c r="AG2" s="176"/>
+      <c r="AI2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="175"/>
+      <c r="AK2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -11974,15 +11974,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12004,29 +12004,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12048,27 +12048,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12090,27 +12090,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12402,6 +12402,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12410,11 +12415,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12490,7 +12490,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12586,19 +12586,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
-      <c r="AL2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="163"/>
-      <c r="AN2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
+      <c r="AL2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -13960,15 +13960,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14002,15 +14002,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14044,15 +14044,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14086,15 +14086,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14472,7 +14472,7 @@
       <c r="AE1" s="181"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14565,19 +14565,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
-      <c r="AK2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="163"/>
-      <c r="AM2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
+      <c r="AK2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="175"/>
+      <c r="AM2" s="176"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15898,15 +15898,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15940,15 +15940,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -15982,15 +15982,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16024,15 +16024,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16324,6 +16324,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16331,11 +16336,6 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16408,7 +16408,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16504,14 +16504,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17782,15 +17782,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17812,29 +17812,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17856,27 +17856,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17898,27 +17898,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18210,18 +18210,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AB19:AH21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18257,42 +18257,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="179" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
+      <c r="A1" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18385,14 +18385,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19626,15 +19626,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19661,15 +19661,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19696,15 +19696,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19731,15 +19731,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20115,7 +20115,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20211,14 +20211,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21518,15 +21518,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21553,15 +21553,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21588,15 +21588,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21623,15 +21623,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -22006,7 +22006,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22102,14 +22102,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="163"/>
-      <c r="AJ2" s="164"/>
+      <c r="AH2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="175"/>
+      <c r="AJ2" s="176"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="178"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23379,15 +23379,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="165" t="s">
+      <c r="F19" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165" t="s">
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="165"/>
+      <c r="J19" s="177"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23409,29 +23409,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="169" t="s">
+      <c r="AB19" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="170"/>
-      <c r="AH19" s="171"/>
+      <c r="AC19" s="164"/>
+      <c r="AD19" s="164"/>
+      <c r="AE19" s="164"/>
+      <c r="AF19" s="164"/>
+      <c r="AG19" s="164"/>
+      <c r="AH19" s="165"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="160" t="s">
+      <c r="F20" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="161"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="161" t="s">
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="161"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23453,27 +23453,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="172"/>
-      <c r="AC20" s="173"/>
-      <c r="AD20" s="173"/>
-      <c r="AE20" s="173"/>
-      <c r="AF20" s="173"/>
-      <c r="AG20" s="173"/>
-      <c r="AH20" s="174"/>
+      <c r="AB20" s="166"/>
+      <c r="AC20" s="167"/>
+      <c r="AD20" s="167"/>
+      <c r="AE20" s="167"/>
+      <c r="AF20" s="167"/>
+      <c r="AG20" s="167"/>
+      <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23495,27 +23495,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="176"/>
-      <c r="AD21" s="176"/>
-      <c r="AE21" s="176"/>
-      <c r="AF21" s="176"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="177"/>
+      <c r="AB21" s="169"/>
+      <c r="AC21" s="170"/>
+      <c r="AD21" s="170"/>
+      <c r="AE21" s="170"/>
+      <c r="AF21" s="170"/>
+      <c r="AG21" s="170"/>
+      <c r="AH21" s="171"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23893,7 +23893,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="167">
+      <c r="A2" s="161">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -23986,14 +23986,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="162" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="163"/>
-      <c r="AI2" s="164"/>
+      <c r="AG2" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="168"/>
+      <c r="A3" s="162"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25314,15 +25314,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165" t="s">
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="165"/>
+      <c r="J20" s="177"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25344,29 +25344,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="169" t="s">
+      <c r="AB20" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="171"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
+      <c r="AF20" s="164"/>
+      <c r="AG20" s="164"/>
+      <c r="AH20" s="165"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="160" t="s">
+      <c r="F21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161" t="s">
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="161"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25388,27 +25388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="172"/>
-      <c r="AC21" s="173"/>
-      <c r="AD21" s="173"/>
-      <c r="AE21" s="173"/>
-      <c r="AF21" s="173"/>
-      <c r="AG21" s="173"/>
-      <c r="AH21" s="174"/>
+      <c r="AB21" s="166"/>
+      <c r="AC21" s="167"/>
+      <c r="AD21" s="167"/>
+      <c r="AE21" s="167"/>
+      <c r="AF21" s="167"/>
+      <c r="AG21" s="167"/>
+      <c r="AH21" s="168"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161" t="s">
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="161"/>
+      <c r="J22" s="173"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25430,27 +25430,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="175"/>
-      <c r="AC22" s="176"/>
-      <c r="AD22" s="176"/>
-      <c r="AE22" s="176"/>
-      <c r="AF22" s="176"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="177"/>
+      <c r="AB22" s="169"/>
+      <c r="AC22" s="170"/>
+      <c r="AD22" s="170"/>
+      <c r="AE22" s="170"/>
+      <c r="AF22" s="170"/>
+      <c r="AG22" s="170"/>
+      <c r="AH22" s="171"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="160" t="s">
+      <c r="F23" s="172" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="161"/>
+      <c r="J23" s="173"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25833,15 +25833,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64cef5f809c20957e1bed8db4fd8bd69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9eb64a58f9f8c69f3f340dcbb635673" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26082,14 +26073,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-19 18:45:13 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2039,6 +2039,24 @@
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2075,31 +2093,13 @@
     <xf numFmtId="0" fontId="24" fillId="25" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2736,43 +2736,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="160"/>
-      <c r="L1" s="160"/>
-      <c r="M1" s="160"/>
-      <c r="N1" s="160"/>
-      <c r="O1" s="160"/>
-      <c r="P1" s="160"/>
-      <c r="Q1" s="160"/>
-      <c r="R1" s="160"/>
-      <c r="S1" s="160"/>
-      <c r="T1" s="160"/>
-      <c r="U1" s="160"/>
-      <c r="V1" s="160"/>
-      <c r="W1" s="160"/>
-      <c r="X1" s="160"/>
-      <c r="Y1" s="160"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="160"/>
-      <c r="AB1" s="160"/>
-      <c r="AC1" s="160"/>
-      <c r="AD1" s="160"/>
-      <c r="AE1" s="160"/>
-      <c r="AF1" s="160"/>
+      <c r="A1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+      <c r="AF1" s="166"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45658</v>
       </c>
       <c r="B2" s="29">
@@ -2868,19 +2868,19 @@
       <c r="AF2" s="39">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
-      <c r="AL2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="175"/>
-      <c r="AN2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
@@ -4230,15 +4230,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -4260,29 +4260,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -4304,27 +4304,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -4346,27 +4346,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -4658,12 +4658,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="AB19:AH21"/>
@@ -4671,6 +4665,12 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4743,7 +4743,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45931</v>
       </c>
       <c r="B2" s="36">
@@ -4839,14 +4839,14 @@
       <c r="AF2" s="36">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
@@ -6222,15 +6222,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -6257,15 +6257,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -6292,15 +6292,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -6327,15 +6327,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -6709,7 +6709,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45962</v>
       </c>
       <c r="B2" s="28">
@@ -6802,14 +6802,14 @@
       <c r="AE2" s="19">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
@@ -8146,15 +8146,15 @@
     <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -8181,15 +8181,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -8216,15 +8216,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -8251,15 +8251,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -8578,8 +8578,8 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="N21" sqref="N21"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AJ4" sqref="AJ4:AJ11"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -8634,7 +8634,7 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45992</v>
       </c>
       <c r="B2" s="28">
@@ -8730,14 +8730,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
@@ -8911,11 +8911,11 @@
       <c r="W4" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y4" s="72" t="s">
-        <v>20</v>
+      <c r="X4" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="83" t="s">
+        <v>26</v>
       </c>
       <c r="Z4" s="157" t="s">
         <v>15</v>
@@ -8944,11 +8944,11 @@
       </c>
       <c r="AI4" s="1">
         <f>COUNTIF(B4:AF4,"U")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" ref="AJ4:AJ11" si="0">AH4-AI4</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1">
@@ -8997,14 +8997,14 @@
       <c r="O5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="72" t="s">
-        <v>20</v>
+      <c r="P5" s="87" t="s">
+        <v>23</v>
       </c>
       <c r="Q5" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="72" t="s">
-        <v>20</v>
+      <c r="R5" s="87" t="s">
+        <v>23</v>
       </c>
       <c r="S5" s="72" t="s">
         <v>20</v>
@@ -9333,8 +9333,8 @@
       <c r="Q8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="R8" s="81" t="s">
-        <v>21</v>
+      <c r="R8" s="72" t="s">
+        <v>20</v>
       </c>
       <c r="S8" s="81" t="s">
         <v>21</v>
@@ -9922,7 +9922,7 @@
       </c>
       <c r="R14" s="70">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14" s="70">
         <f t="shared" si="5"/>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="P15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="70">
         <f t="shared" si="6"/>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="R15" s="70">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S15" s="70">
         <f t="shared" si="6"/>
@@ -10113,15 +10113,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -10143,29 +10143,29 @@
       <c r="W20" s="48"/>
       <c r="X20" s="48"/>
       <c r="Y20" s="49"/>
-      <c r="AB20" s="163" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -10187,27 +10187,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -10229,27 +10229,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
-      <c r="AB22" s="169"/>
-      <c r="AC22" s="170"/>
-      <c r="AD22" s="170"/>
-      <c r="AE22" s="170"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="170"/>
-      <c r="AH22" s="171"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -10592,40 +10592,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="179"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="179"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45689</v>
       </c>
       <c r="B2" s="55">
@@ -10712,19 +10712,19 @@
       <c r="AC2" s="37">
         <v>28</v>
       </c>
-      <c r="AE2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="175"/>
-      <c r="AG2" s="176"/>
-      <c r="AI2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="175"/>
-      <c r="AK2" s="176"/>
+      <c r="AE2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="163"/>
+      <c r="AG2" s="164"/>
+      <c r="AI2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="163"/>
+      <c r="AK2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
@@ -11974,15 +11974,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -12004,29 +12004,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -12048,27 +12048,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -12090,27 +12090,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -12402,11 +12402,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -12415,6 +12410,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AC14">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
@@ -12490,7 +12490,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45717</v>
       </c>
       <c r="B2" s="41">
@@ -12586,19 +12586,19 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
-      <c r="AL2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="175"/>
-      <c r="AN2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
+      <c r="AL2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="163"/>
+      <c r="AN2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="41" t="s">
         <v>6</v>
       </c>
@@ -13960,15 +13960,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -14002,15 +14002,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -14044,15 +14044,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -14086,15 +14086,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -14472,7 +14472,7 @@
       <c r="AE1" s="181"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45748</v>
       </c>
       <c r="B2" s="36">
@@ -14565,19 +14565,19 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
-      <c r="AK2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="175"/>
-      <c r="AM2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
+      <c r="AK2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="163"/>
+      <c r="AM2" s="164"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
@@ -15898,15 +15898,15 @@
     </row>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -15940,15 +15940,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -15982,15 +15982,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -16024,15 +16024,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -16324,11 +16324,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -16336,6 +16331,11 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AE14">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -16408,7 +16408,7 @@
       <c r="AF1" s="181"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45778</v>
       </c>
       <c r="B2" s="28">
@@ -16504,14 +16504,14 @@
       <c r="AF2" s="19">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
@@ -17782,15 +17782,15 @@
     <row r="18" spans="5:34" ht="15" customHeight="1" thickBot="1"/>
     <row r="19" spans="5:34" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -17812,29 +17812,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34" ht="15" customHeight="1">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -17856,27 +17856,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -17898,27 +17898,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -18210,18 +18210,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:AF14">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
@@ -18257,42 +18257,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="179"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="179"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
-      <c r="AC1" s="179"/>
-      <c r="AD1" s="179"/>
-      <c r="AE1" s="179"/>
+      <c r="A1" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="180"/>
+      <c r="AB1" s="180"/>
+      <c r="AC1" s="180"/>
+      <c r="AD1" s="180"/>
+      <c r="AE1" s="180"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45809</v>
       </c>
       <c r="B2" s="19">
@@ -18385,14 +18385,14 @@
       <c r="AE2" s="37">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -19626,15 +19626,15 @@
     <row r="18" spans="5:25" ht="15" customHeight="1"/>
     <row r="19" spans="5:25" ht="15" customHeight="1">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -19661,15 +19661,15 @@
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -19696,15 +19696,15 @@
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -19731,15 +19731,15 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -20115,7 +20115,7 @@
       <c r="AF1" s="56"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45839</v>
       </c>
       <c r="B2" s="37">
@@ -20211,14 +20211,14 @@
       <c r="AF2" s="37">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
@@ -21518,15 +21518,15 @@
     </row>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="7" t="s">
         <v>17</v>
@@ -21553,15 +21553,15 @@
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="31" t="s">
         <v>42</v>
@@ -21588,15 +21588,15 @@
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="27" t="s">
         <v>15</v>
@@ -21623,15 +21623,15 @@
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="8" t="s">
         <v>26</v>
@@ -21949,7 +21949,7 @@
   <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AC14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -22006,7 +22006,7 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45870</v>
       </c>
       <c r="B2" s="38">
@@ -22102,14 +22102,14 @@
       <c r="AF2" s="55">
         <v>31</v>
       </c>
-      <c r="AH2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="175"/>
-      <c r="AJ2" s="176"/>
+      <c r="AH2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="164"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="180"/>
+      <c r="A3" s="178"/>
       <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
@@ -23379,15 +23379,15 @@
     <row r="18" spans="5:34" ht="15" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177" t="s">
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="177"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="59"/>
       <c r="N19" s="7" t="s">
         <v>17</v>
@@ -23409,29 +23409,29 @@
       <c r="W19" s="48"/>
       <c r="X19" s="48"/>
       <c r="Y19" s="49"/>
-      <c r="AB19" s="163" t="s">
+      <c r="AB19" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC19" s="164"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="164"/>
-      <c r="AF19" s="164"/>
-      <c r="AG19" s="164"/>
-      <c r="AH19" s="165"/>
+      <c r="AC19" s="170"/>
+      <c r="AD19" s="170"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="170"/>
+      <c r="AG19" s="170"/>
+      <c r="AH19" s="171"/>
     </row>
     <row r="20" spans="5:34">
       <c r="E20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="172" t="s">
+      <c r="F20" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173" t="s">
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="173"/>
+      <c r="J20" s="161"/>
       <c r="K20" s="59"/>
       <c r="N20" s="31" t="s">
         <v>42</v>
@@ -23453,27 +23453,27 @@
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="46"/>
-      <c r="AB20" s="166"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="168"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
+      <c r="AH20" s="174"/>
     </row>
     <row r="21" spans="5:34" ht="15" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="27" t="s">
         <v>15</v>
@@ -23495,27 +23495,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="46"/>
-      <c r="AB21" s="169"/>
-      <c r="AC21" s="170"/>
-      <c r="AD21" s="170"/>
-      <c r="AE21" s="170"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="170"/>
-      <c r="AH21" s="171"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="176"/>
+      <c r="AD21" s="176"/>
+      <c r="AE21" s="176"/>
+      <c r="AF21" s="176"/>
+      <c r="AG21" s="176"/>
+      <c r="AH21" s="177"/>
     </row>
     <row r="22" spans="5:34">
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="8" t="s">
         <v>26</v>
@@ -23838,7 +23838,7 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AH6" sqref="AH6"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
@@ -23893,7 +23893,7 @@
       <c r="AI1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="161">
+      <c r="A2" s="167">
         <v>45901</v>
       </c>
       <c r="B2" s="38">
@@ -23986,14 +23986,14 @@
       <c r="AE2" s="38">
         <v>30</v>
       </c>
-      <c r="AG2" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="175"/>
-      <c r="AI2" s="176"/>
+      <c r="AG2" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="164"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="162"/>
+      <c r="A3" s="168"/>
       <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
@@ -25314,15 +25314,15 @@
     <row r="19" spans="5:34" ht="15" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="177"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="177" t="s">
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="177"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="59"/>
       <c r="N20" s="99" t="s">
         <v>17</v>
@@ -25344,29 +25344,29 @@
       <c r="W20" s="104"/>
       <c r="X20" s="104"/>
       <c r="Y20" s="105"/>
-      <c r="AB20" s="163" t="s">
+      <c r="AB20" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="AC20" s="164"/>
-      <c r="AD20" s="164"/>
-      <c r="AE20" s="164"/>
-      <c r="AF20" s="164"/>
-      <c r="AG20" s="164"/>
-      <c r="AH20" s="165"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="171"/>
     </row>
     <row r="21" spans="5:34">
       <c r="E21" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="172" t="s">
+      <c r="F21" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173" t="s">
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="173"/>
+      <c r="J21" s="161"/>
       <c r="K21" s="59"/>
       <c r="N21" s="106" t="s">
         <v>42</v>
@@ -25388,27 +25388,27 @@
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
       <c r="Y21" s="107"/>
-      <c r="AB21" s="166"/>
-      <c r="AC21" s="167"/>
-      <c r="AD21" s="167"/>
-      <c r="AE21" s="167"/>
-      <c r="AF21" s="167"/>
-      <c r="AG21" s="167"/>
-      <c r="AH21" s="168"/>
+      <c r="AB21" s="172"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
+      <c r="AH21" s="174"/>
     </row>
     <row r="22" spans="5:34" ht="15" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="172" t="s">
+      <c r="F22" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173" t="s">
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="173"/>
+      <c r="J22" s="161"/>
       <c r="K22" s="59"/>
       <c r="N22" s="80" t="s">
         <v>15</v>
@@ -25430,27 +25430,27 @@
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="107"/>
-      <c r="AB22" s="169"/>
-      <c r="AC22" s="170"/>
-      <c r="AD22" s="170"/>
-      <c r="AE22" s="170"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="170"/>
-      <c r="AH22" s="171"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="176"/>
+      <c r="AD22" s="176"/>
+      <c r="AE22" s="176"/>
+      <c r="AF22" s="176"/>
+      <c r="AG22" s="176"/>
+      <c r="AH22" s="177"/>
     </row>
     <row r="23" spans="5:34">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="172" t="s">
+      <c r="F23" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173" t="s">
+      <c r="G23" s="161"/>
+      <c r="H23" s="161"/>
+      <c r="I23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="173"/>
+      <c r="J23" s="161"/>
       <c r="K23" s="59"/>
       <c r="N23" s="108" t="s">
         <v>26</v>
@@ -25833,6 +25833,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64cef5f809c20957e1bed8db4fd8bd69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9eb64a58f9f8c69f3f340dcbb635673" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -26073,23 +26082,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25036EC1-2728-4BE7-AC17-163F56A6F287}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501C7360-5CDC-4DE3-A5FC-A409AA8E5DCA}"/>
 </file>
</xml_diff>

<commit_message>
Update files and calendar (2025-12-29 18:45:39 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2025.xlsx
+++ b/files/IT_2025.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29622"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Gdj7YK5Ag6v7y/4fR5tXwO/rpvJdszXS8v31P2EpceMXbAZlXLrSauO60gFaVasDUgoVoHqkdXqW+ZXZBvlILQ==" saltValue="hCk+xaV8/orzhcg23K2gmg==" spinCount="100000"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lufthansagroup.sharepoint.com/sites/LGSPITTopics/Shared Documents/Horarios Service Center/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{0DD657E5-C989-47DA-8F3B-2B5A17B9AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{7164E94B-322B-4F74-B4DB-8B6D9D3B7C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN25" sheetId="68" r:id="rId1"/>
@@ -2722,7 +2722,7 @@
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -3839,8 +3839,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="15" thickBot="1"/>
-    <row r="12" spans="1:40" ht="15" thickBot="1">
+    <row r="11" spans="1:40" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:40" ht="15.75" thickBot="1">
       <c r="A12" s="67" t="s">
         <v>31</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="15" thickBot="1">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1">
       <c r="A13" s="69" t="s">
         <v>32</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:34" ht="15" thickBot="1"/>
+    <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
       <c r="F19" s="165" t="s">
@@ -4312,7 +4312,7 @@
       <c r="AG20" s="173"/>
       <c r="AH20" s="174"/>
     </row>
-    <row r="21" spans="5:34" ht="15" thickBot="1">
+    <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
@@ -4634,7 +4634,7 @@
       <c r="X32" s="18"/>
       <c r="Y32" s="46"/>
     </row>
-    <row r="33" spans="14:25" ht="15" thickBot="1">
+    <row r="33" spans="14:25" ht="15.75" thickBot="1">
       <c r="N33" s="14" t="s">
         <v>86</v>
       </c>
@@ -4687,13 +4687,13 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AC26" sqref="AC26"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AL23" sqref="AL23"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -5710,7 +5710,7 @@
       </c>
       <c r="AH10" s="1">
         <f>'SEP25'!AI10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AI10" s="1">
         <f>COUNTIF(B10:AF10,"U")</f>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="AJ10" s="1">
         <f t="shared" ref="AJ10" si="2">AH10-AI10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="15" customHeight="1">
@@ -5831,8 +5831,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="15" thickBot="1"/>
-    <row r="13" spans="1:36" ht="15" thickBot="1">
+    <row r="12" spans="1:36" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:36" ht="15.75" thickBot="1">
       <c r="A13" s="67" t="s">
         <v>31</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15" thickBot="1">
+    <row r="14" spans="1:36" ht="15.75" thickBot="1">
       <c r="A14" s="69" t="s">
         <v>32</v>
       </c>
@@ -6219,7 +6219,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
       <c r="F20" s="165" t="s">
@@ -6323,7 +6322,7 @@
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
     </row>
-    <row r="23" spans="5:25" ht="15">
+    <row r="23" spans="5:25">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
@@ -6603,7 +6602,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="46"/>
     </row>
-    <row r="34" spans="14:25" ht="15" thickBot="1">
+    <row r="34" spans="14:25" ht="15.75" thickBot="1">
       <c r="N34" s="14" t="s">
         <v>86</v>
       </c>
@@ -6654,13 +6653,13 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="32" width="6.7109375" customWidth="1"/>
@@ -7649,7 +7648,7 @@
       </c>
       <c r="AG10" s="1">
         <f>'OCT25'!AJ10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AH10" s="1">
         <f>COUNTIF(B10:AE10,"U")</f>
@@ -7657,7 +7656,7 @@
       </c>
       <c r="AI10" s="1">
         <f t="shared" ref="AI10" si="3">AG10-AH10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="15" customHeight="1">
@@ -7767,8 +7766,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" thickBot="1"/>
-    <row r="13" spans="1:35" ht="15" thickBot="1">
+    <row r="12" spans="1:35" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:35" ht="15.75" thickBot="1">
       <c r="A13" s="67" t="s">
         <v>31</v>
       </c>
@@ -7893,7 +7892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15" thickBot="1">
+    <row r="14" spans="1:35" ht="15.75" thickBot="1">
       <c r="A14" s="69" t="s">
         <v>32</v>
       </c>
@@ -8143,7 +8142,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:25" ht="15"/>
     <row r="20" spans="5:25" ht="14.45" customHeight="1">
       <c r="E20" s="5"/>
       <c r="F20" s="165" t="s">
@@ -8247,7 +8245,7 @@
       <c r="X22" s="18"/>
       <c r="Y22" s="46"/>
     </row>
-    <row r="23" spans="5:25" ht="15">
+    <row r="23" spans="5:25">
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
@@ -8527,7 +8525,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="46"/>
     </row>
-    <row r="34" spans="14:25" ht="15" thickBot="1">
+    <row r="34" spans="14:25" ht="15.75" thickBot="1">
       <c r="N34" s="14" t="s">
         <v>103</v>
       </c>
@@ -8578,13 +8576,13 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AJ4" sqref="AJ4:AJ11"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="W10" sqref="W10"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -9570,7 +9568,7 @@
         <v>26</v>
       </c>
       <c r="W10" s="83" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>17</v>
@@ -9600,16 +9598,15 @@
         <v>23</v>
       </c>
       <c r="AH10" s="1">
-        <f>'NOV25'!AI10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AI10" s="1">
         <f t="shared" ref="AI10" si="2">COUNTIF(B10:AF10,"U")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AJ10" s="1">
         <f t="shared" ref="AJ10" si="3">AH10-AI10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="15" customHeight="1">
@@ -9722,8 +9719,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="15" thickBot="1"/>
-    <row r="13" spans="1:36" ht="15" thickBot="1">
+    <row r="12" spans="1:36" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:36" ht="15.75" thickBot="1">
       <c r="A13" s="67" t="s">
         <v>31</v>
       </c>
@@ -9852,7 +9849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15" thickBot="1">
+    <row r="14" spans="1:36" ht="15.75" thickBot="1">
       <c r="A14" s="69" t="s">
         <v>32</v>
       </c>
@@ -10110,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:34" ht="15" thickBot="1"/>
+    <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34" ht="15.75" customHeight="1">
       <c r="E20" s="5"/>
       <c r="F20" s="165" t="s">
@@ -10195,7 +10192,7 @@
       <c r="AG21" s="173"/>
       <c r="AH21" s="174"/>
     </row>
-    <row r="22" spans="5:34" ht="15" thickBot="1">
+    <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
@@ -10517,7 +10514,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="46"/>
     </row>
-    <row r="34" spans="14:25" ht="15" thickBot="1">
+    <row r="34" spans="14:25" ht="15.75" thickBot="1">
       <c r="N34" s="14" t="s">
         <v>86</v>
       </c>
@@ -10578,7 +10575,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="30" width="6.7109375" customWidth="1"/>
@@ -11619,8 +11616,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" thickBot="1"/>
-    <row r="12" spans="1:37" ht="15" thickBot="1">
+    <row r="11" spans="1:37" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:37" ht="15.75" thickBot="1">
       <c r="A12" s="67" t="s">
         <v>31</v>
       </c>
@@ -11737,7 +11734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" thickBot="1">
+    <row r="13" spans="1:37" ht="15.75" thickBot="1">
       <c r="A13" s="69" t="s">
         <v>32</v>
       </c>
@@ -11971,7 +11968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:34" ht="15" thickBot="1"/>
+    <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
       <c r="F19" s="165" t="s">
@@ -12056,7 +12053,7 @@
       <c r="AG20" s="173"/>
       <c r="AH20" s="174"/>
     </row>
-    <row r="21" spans="5:34" ht="15" thickBot="1">
+    <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
@@ -12440,7 +12437,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -13565,8 +13562,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="15" thickBot="1"/>
-    <row r="12" spans="1:40" ht="15" thickBot="1">
+    <row r="11" spans="1:40" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:40" ht="15.75" thickBot="1">
       <c r="A12" s="67" t="s">
         <v>31</v>
       </c>
@@ -13695,7 +13692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="15" thickBot="1">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1">
       <c r="A13" s="69" t="s">
         <v>32</v>
       </c>
@@ -14362,7 +14359,7 @@
       <c r="X32" s="18"/>
       <c r="Y32" s="46"/>
     </row>
-    <row r="33" spans="14:25" ht="15" thickBot="1">
+    <row r="33" spans="14:25" ht="15.75" thickBot="1">
       <c r="N33" s="14" t="s">
         <v>86</v>
       </c>
@@ -14423,7 +14420,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="32" width="6.7109375" customWidth="1"/>
@@ -15520,8 +15517,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" thickBot="1"/>
-    <row r="12" spans="1:39" ht="15" thickBot="1">
+    <row r="11" spans="1:39" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:39" ht="15.75" thickBot="1">
       <c r="A12" s="67" t="s">
         <v>31</v>
       </c>
@@ -15646,7 +15643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" thickBot="1">
+    <row r="13" spans="1:39" ht="15.75" thickBot="1">
       <c r="A13" s="69" t="s">
         <v>32</v>
       </c>
@@ -16362,7 +16359,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -17864,7 +17861,7 @@
       <c r="AG20" s="173"/>
       <c r="AH20" s="174"/>
     </row>
-    <row r="21" spans="5:34" ht="15" thickBot="1">
+    <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
@@ -18186,7 +18183,7 @@
       <c r="X32" s="18"/>
       <c r="Y32" s="46"/>
     </row>
-    <row r="33" spans="14:25" ht="15" thickBot="1">
+    <row r="33" spans="14:25" ht="15.75" thickBot="1">
       <c r="N33" s="14" t="s">
         <v>86</v>
       </c>
@@ -18247,7 +18244,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="32" width="6.7109375" customWidth="1"/>
@@ -20007,7 +20004,7 @@
       <c r="X32" s="18"/>
       <c r="Y32" s="46"/>
     </row>
-    <row r="33" spans="14:25" ht="15" thickBot="1">
+    <row r="33" spans="14:25" ht="15.75" thickBot="1">
       <c r="N33" s="14" t="s">
         <v>86</v>
       </c>
@@ -20068,7 +20065,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -21128,8 +21125,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" thickBot="1"/>
-    <row r="13" spans="1:37" ht="15" thickBot="1">
+    <row r="12" spans="1:37" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:37" ht="15.75" thickBot="1">
       <c r="A13" s="67" t="s">
         <v>31</v>
       </c>
@@ -21258,7 +21255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" thickBot="1">
+    <row r="14" spans="1:37" ht="15.75" thickBot="1">
       <c r="A14" s="69" t="s">
         <v>32</v>
       </c>
@@ -21898,7 +21895,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="46"/>
     </row>
-    <row r="34" spans="14:25" ht="15" thickBot="1">
+    <row r="34" spans="14:25" ht="15.75" thickBot="1">
       <c r="N34" s="14" t="s">
         <v>86</v>
       </c>
@@ -21949,13 +21946,13 @@
   <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="33" width="6.7109375" customWidth="1"/>
@@ -22988,8 +22985,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="15" thickBot="1"/>
-    <row r="12" spans="1:40" ht="15" thickBot="1">
+    <row r="11" spans="1:40" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:40" ht="15.75" thickBot="1">
       <c r="A12" s="67" t="s">
         <v>31</v>
       </c>
@@ -23118,7 +23115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="15" thickBot="1">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1">
       <c r="A13" s="69" t="s">
         <v>32</v>
       </c>
@@ -23376,7 +23373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:34" ht="15" thickBot="1"/>
+    <row r="18" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="19" spans="5:34">
       <c r="E19" s="5"/>
       <c r="F19" s="165" t="s">
@@ -23461,7 +23458,7 @@
       <c r="AG20" s="173"/>
       <c r="AH20" s="174"/>
     </row>
-    <row r="21" spans="5:34" ht="15" thickBot="1">
+    <row r="21" spans="5:34" ht="15.75" thickBot="1">
       <c r="E21" s="61" t="s">
         <v>16</v>
       </c>
@@ -23783,7 +23780,7 @@
       <c r="X32" s="18"/>
       <c r="Y32" s="46"/>
     </row>
-    <row r="33" spans="14:25" ht="15" thickBot="1">
+    <row r="33" spans="14:25" ht="15.75" thickBot="1">
       <c r="N33" s="14" t="s">
         <v>86</v>
       </c>
@@ -23838,13 +23835,13 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AH6" sqref="AH6"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AI16" sqref="AI16"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="32" width="6.7109375" customWidth="1"/>
@@ -24831,8 +24828,7 @@
         <v>21</v>
       </c>
       <c r="AG10" s="1">
-        <f>'AUG25'!AJ8</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AH10" s="1">
         <f>COUNTIF(B10:AE10,"U")</f>
@@ -24840,7 +24836,7 @@
       </c>
       <c r="AI10" s="1">
         <f t="shared" ref="AI10" si="2">AG10-AH10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="15" customHeight="1">
@@ -24935,8 +24931,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" thickBot="1"/>
-    <row r="13" spans="1:35" ht="15" thickBot="1">
+    <row r="12" spans="1:35" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:35" ht="15.75" thickBot="1">
       <c r="A13" s="67" t="s">
         <v>31</v>
       </c>
@@ -25061,7 +25057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15" thickBot="1">
+    <row r="14" spans="1:35" ht="15.75" thickBot="1">
       <c r="A14" s="69" t="s">
         <v>32</v>
       </c>
@@ -25311,7 +25307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:34" ht="15" thickBot="1"/>
+    <row r="19" spans="5:34" ht="15.75" thickBot="1"/>
     <row r="20" spans="5:34">
       <c r="E20" s="5"/>
       <c r="F20" s="165" t="s">
@@ -25396,7 +25392,7 @@
       <c r="AG21" s="173"/>
       <c r="AH21" s="174"/>
     </row>
-    <row r="22" spans="5:34" ht="15" thickBot="1">
+    <row r="22" spans="5:34" ht="15.75" thickBot="1">
       <c r="E22" s="61" t="s">
         <v>16</v>
       </c>
@@ -25732,7 +25728,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="107"/>
     </row>
-    <row r="34" spans="14:25" ht="15" thickBot="1">
+    <row r="34" spans="14:25" ht="15.75" thickBot="1">
       <c r="N34" s="118" t="s">
         <v>86</v>
       </c>

</xml_diff>